<commit_message>
Add new hero death knight class
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentutsedu-my.sharepoint.com/personal/daoyu_shen_uts_edu_au/Documents/UTS/7. Python Space/Legends of Champions Tactics/Legends of Champions Tactics_exe_1.0_A/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_134183789C06D3CCA887A5464D29A400CB4964CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7162B24-A325-4CD8-A413-535B06633497}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3F6DB1-A0CD-4D84-9462-E2CE71CEA05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bar" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>Warlock_Destruction</t>
   </si>
   <si>
-    <t>Death Knight_Comprehensiveness</t>
-  </si>
-  <si>
     <t>Hp_Max</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Death Knight_Frost</t>
   </si>
 </sst>
 </file>
@@ -1681,7 +1681,7 @@
   </sheetPr>
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29892,7 +29892,10 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29900,15 +29903,16 @@
     <col min="1" max="1" width="36.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.88671875" customWidth="1"/>
     <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.21875" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="26.33203125" customWidth="1"/>
     <col min="8" max="8" width="27.44140625" customWidth="1"/>
     <col min="9" max="13" width="31" customWidth="1"/>
     <col min="14" max="14" width="26.21875" customWidth="1"/>
     <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="17" width="32.77734375" customWidth="1"/>
+    <col min="16" max="16" width="32.77734375" customWidth="1"/>
+    <col min="17" max="17" width="34.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -29959,7 +29963,7 @@
         <v>31</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>8</v>
@@ -29976,7 +29980,7 @@
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2">
         <v>105</v>
@@ -30041,7 +30045,7 @@
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2">
         <v>95</v>
@@ -30191,7 +30195,7 @@
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2">
         <v>75</v>
@@ -30256,7 +30260,7 @@
     </row>
     <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="9">
         <v>65</v>
@@ -30406,7 +30410,7 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="9">
         <v>60</v>
@@ -30471,7 +30475,7 @@
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="9">
         <v>50</v>
@@ -30621,7 +30625,7 @@
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="9">
         <v>20</v>
@@ -30686,7 +30690,7 @@
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="9">
         <v>10</v>
@@ -30836,7 +30840,7 @@
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="9">
         <v>5</v>
@@ -30901,7 +30905,7 @@
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="9">
         <v>-5</v>
@@ -30966,7 +30970,7 @@
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="9">
         <f t="shared" ref="B16:U16" si="4">(B14+B15)/2</f>
@@ -31114,7 +31118,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -31137,9 +31141,9 @@
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="9">
         <f t="shared" ref="B19:U19" si="5">B4+B7+B10+B13+B16+B17</f>

</xml_diff>

<commit_message>
Death Knight Frost finish, Death Knight Plague on going.
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3F6DB1-A0CD-4D84-9462-E2CE71CEA05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5606C801-8B27-4D79-BCC8-C2C011BF6B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Warrior</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Death Knight_Frost</t>
+  </si>
+  <si>
+    <t>Death Knight_Plague</t>
   </si>
 </sst>
 </file>
@@ -2135,19 +2138,19 @@
         <v>105</v>
       </c>
       <c r="J8" s="7">
-        <f>'Property List'!R4</f>
-        <v>75</v>
-      </c>
-      <c r="K8" s="7">
         <f>'Property List'!S4</f>
         <v>75</v>
       </c>
-      <c r="L8" s="7">
+      <c r="K8" s="7">
         <f>'Property List'!T4</f>
         <v>75</v>
       </c>
+      <c r="L8" s="7">
+        <f>'Property List'!U4</f>
+        <v>75</v>
+      </c>
       <c r="M8" s="7">
-        <f>'Property List'!U4</f>
+        <f>'Property List'!V4</f>
         <v>75</v>
       </c>
       <c r="N8" s="4">
@@ -2203,19 +2206,19 @@
         <v>65</v>
       </c>
       <c r="J9" s="7">
-        <f>'Property List'!R7</f>
-        <v>75</v>
-      </c>
-      <c r="K9" s="7">
         <f>'Property List'!S7</f>
         <v>75</v>
       </c>
-      <c r="L9" s="7">
+      <c r="K9" s="7">
         <f>'Property List'!T7</f>
         <v>75</v>
       </c>
+      <c r="L9" s="7">
+        <f>'Property List'!U7</f>
+        <v>75</v>
+      </c>
       <c r="M9" s="7">
-        <f>'Property List'!U7</f>
+        <f>'Property List'!V7</f>
         <v>75</v>
       </c>
       <c r="N9" s="4">
@@ -2271,19 +2274,19 @@
         <v>50</v>
       </c>
       <c r="J10" s="7">
-        <f>'Property List'!R10</f>
-        <v>27</v>
-      </c>
-      <c r="K10" s="7">
         <f>'Property List'!S10</f>
         <v>27</v>
       </c>
-      <c r="L10" s="7">
+      <c r="K10" s="7">
         <f>'Property List'!T10</f>
         <v>27</v>
       </c>
+      <c r="L10" s="7">
+        <f>'Property List'!U10</f>
+        <v>27</v>
+      </c>
       <c r="M10" s="7">
-        <f>'Property List'!U10</f>
+        <f>'Property List'!V10</f>
         <v>27</v>
       </c>
       <c r="N10" s="4">
@@ -2339,19 +2342,19 @@
         <v>15</v>
       </c>
       <c r="J11" s="7">
-        <f>'Property List'!R13</f>
-        <v>25</v>
-      </c>
-      <c r="K11" s="7">
         <f>'Property List'!S13</f>
         <v>25</v>
       </c>
-      <c r="L11" s="7">
+      <c r="K11" s="7">
         <f>'Property List'!T13</f>
         <v>25</v>
       </c>
+      <c r="L11" s="7">
+        <f>'Property List'!U13</f>
+        <v>25</v>
+      </c>
       <c r="M11" s="7">
-        <f>'Property List'!U13</f>
+        <f>'Property List'!V13</f>
         <v>25</v>
       </c>
       <c r="N11" s="4">
@@ -2407,19 +2410,19 @@
         <v>31</v>
       </c>
       <c r="J12" s="2">
-        <f>'Property List'!R17</f>
-        <v>34</v>
-      </c>
-      <c r="K12" s="2">
         <f>'Property List'!S17</f>
         <v>34</v>
       </c>
-      <c r="L12" s="2">
+      <c r="K12" s="2">
         <f>'Property List'!T17</f>
         <v>34</v>
       </c>
+      <c r="L12" s="2">
+        <f>'Property List'!U17</f>
+        <v>34</v>
+      </c>
       <c r="M12" s="2">
-        <f>'Property List'!U17</f>
+        <f>'Property List'!V17</f>
         <v>34</v>
       </c>
       <c r="N12" s="4">
@@ -29889,13 +29892,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29911,11 +29914,12 @@
     <col min="9" max="13" width="31" customWidth="1"/>
     <col min="14" max="14" width="26.21875" customWidth="1"/>
     <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="32.77734375" customWidth="1"/>
-    <col min="17" max="17" width="34.77734375" customWidth="1"/>
+    <col min="16" max="16" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>17</v>
@@ -29966,19 +29970,22 @@
         <v>44</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
@@ -30030,8 +30037,8 @@
       <c r="Q2" s="9">
         <v>110</v>
       </c>
-      <c r="R2" s="2">
-        <v>80</v>
+      <c r="R2" s="9">
+        <v>110</v>
       </c>
       <c r="S2" s="2">
         <v>80</v>
@@ -30042,8 +30049,11 @@
       <c r="U2" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V2" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>33</v>
       </c>
@@ -30095,8 +30105,8 @@
       <c r="Q3" s="9">
         <v>100</v>
       </c>
-      <c r="R3" s="2">
-        <v>70</v>
+      <c r="R3" s="9">
+        <v>100</v>
       </c>
       <c r="S3" s="2">
         <v>70</v>
@@ -30107,13 +30117,16 @@
       <c r="U3" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V3" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:U4" si="0">(B2+B3)/2</f>
+        <f t="shared" ref="B4:V4" si="0">(B2+B3)/2</f>
         <v>100</v>
       </c>
       <c r="C4" s="2">
@@ -30177,8 +30190,8 @@
         <v>105</v>
       </c>
       <c r="R4" s="2">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f t="shared" ref="R4" si="1">(R2+R3)/2</f>
+        <v>105</v>
       </c>
       <c r="S4" s="2">
         <f t="shared" si="0"/>
@@ -30192,8 +30205,12 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V4" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
@@ -30245,8 +30262,8 @@
       <c r="Q5" s="9">
         <v>70</v>
       </c>
-      <c r="R5" s="2">
-        <v>80</v>
+      <c r="R5" s="9">
+        <v>70</v>
       </c>
       <c r="S5" s="2">
         <v>80</v>
@@ -30257,8 +30274,11 @@
       <c r="U5" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V5" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
@@ -30311,7 +30331,7 @@
         <v>60</v>
       </c>
       <c r="R6" s="9">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S6" s="9">
         <v>70</v>
@@ -30322,93 +30342,100 @@
       <c r="U6" s="9">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V6" s="9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="9">
-        <f t="shared" ref="B7:U7" si="1">(B5+B6)/2</f>
+        <f t="shared" ref="B7:V7" si="2">(B5+B6)/2</f>
         <v>70</v>
       </c>
       <c r="C7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="D7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="E7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="F7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="I7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="J7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="K7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="L7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="M7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="N7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="O7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="P7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="Q7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="R7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="R7" si="3">(R5+R6)/2</f>
+        <v>65</v>
+      </c>
+      <c r="S7" s="9">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="S7" s="9">
-        <f t="shared" si="1"/>
+      <c r="T7" s="9">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="T7" s="9">
-        <f t="shared" si="1"/>
+      <c r="U7" s="9">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="U7" s="9">
-        <f t="shared" si="1"/>
+      <c r="V7" s="9">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
@@ -30461,7 +30488,7 @@
         <v>55</v>
       </c>
       <c r="R8" s="9">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="S8" s="9">
         <v>30</v>
@@ -30472,8 +30499,11 @@
       <c r="U8" s="9">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
@@ -30526,7 +30556,7 @@
         <v>45</v>
       </c>
       <c r="R9" s="9">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="S9" s="9">
         <v>24</v>
@@ -30537,93 +30567,100 @@
       <c r="U9" s="9">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V9" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <f t="shared" ref="B10:U10" si="2">(B8+B9)/2</f>
+        <f t="shared" ref="B10:V10" si="4">(B8+B9)/2</f>
         <v>55</v>
       </c>
       <c r="C10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="E10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="I10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="J10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="K10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="L10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="M10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="N10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="O10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="P10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="Q10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="R10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="R10" si="5">(R8+R9)/2</f>
+        <v>50</v>
+      </c>
+      <c r="S10" s="9">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="S10" s="9">
-        <f t="shared" si="2"/>
+      <c r="T10" s="9">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="T10" s="9">
-        <f t="shared" si="2"/>
+      <c r="U10" s="9">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="U10" s="9">
-        <f t="shared" si="2"/>
+      <c r="V10" s="9">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>38</v>
       </c>
@@ -30676,7 +30713,7 @@
         <v>20</v>
       </c>
       <c r="R11" s="9">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="S11" s="9">
         <v>30</v>
@@ -30687,8 +30724,11 @@
       <c r="U11" s="9">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V11" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
@@ -30741,7 +30781,7 @@
         <v>10</v>
       </c>
       <c r="R12" s="9">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="S12" s="9">
         <v>20</v>
@@ -30752,93 +30792,100 @@
       <c r="U12" s="9">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V12" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="9">
-        <f t="shared" ref="B13:U13" si="3">(B11+B12)/2</f>
+        <f t="shared" ref="B13:V13" si="6">(B11+B12)/2</f>
         <v>15</v>
       </c>
       <c r="C13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="E13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="F13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="G13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="I13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="J13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="L13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="M13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="N13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="O13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="P13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="Q13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="R13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="R13" si="7">(R11+R12)/2</f>
+        <v>15</v>
+      </c>
+      <c r="S13" s="9">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="S13" s="9">
-        <f t="shared" si="3"/>
+      <c r="T13" s="9">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="T13" s="9">
-        <f t="shared" si="3"/>
+      <c r="U13" s="9">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="U13" s="9">
-        <f t="shared" si="3"/>
+      <c r="V13" s="9">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>40</v>
       </c>
@@ -30902,8 +30949,11 @@
       <c r="U14" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V14" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>41</v>
       </c>
@@ -30967,93 +31017,100 @@
       <c r="U15" s="9">
         <v>-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V15" s="9">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="9">
-        <f t="shared" ref="B16:U16" si="4">(B14+B15)/2</f>
+        <f t="shared" ref="B16:V16" si="8">(B14+B15)/2</f>
         <v>0</v>
       </c>
       <c r="C16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="R16" si="9">(R14+R15)/2</f>
         <v>0</v>
       </c>
       <c r="S16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V16" s="9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
@@ -31106,7 +31163,7 @@
         <v>31</v>
       </c>
       <c r="R17" s="9">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="S17" s="9">
         <v>34</v>
@@ -31117,8 +31174,11 @@
       <c r="U17" s="9">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="V17" s="9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -31140,89 +31200,94 @@
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
-    </row>
-    <row r="19" spans="1:21" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="V18" s="9"/>
+    </row>
+    <row r="19" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="9">
-        <f t="shared" ref="B19:U19" si="5">B4+B7+B10+B13+B16+B17</f>
+        <f t="shared" ref="B19:V19" si="10">B4+B7+B10+B13+B16+B17</f>
         <v>265</v>
       </c>
       <c r="C19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>204</v>
       </c>
       <c r="D19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>199</v>
       </c>
       <c r="E19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>266</v>
       </c>
       <c r="F19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>261</v>
       </c>
       <c r="G19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
       <c r="H19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>244</v>
       </c>
       <c r="I19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>244</v>
       </c>
       <c r="J19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>244</v>
       </c>
       <c r="K19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>244</v>
       </c>
       <c r="L19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>244</v>
       </c>
       <c r="M19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>246</v>
       </c>
       <c r="N19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>251</v>
       </c>
       <c r="O19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>251</v>
       </c>
       <c r="P19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>251</v>
       </c>
       <c r="Q19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>266</v>
       </c>
       <c r="R19" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="R19" si="11">R4+R7+R10+R13+R16+R17</f>
+        <v>266</v>
+      </c>
+      <c r="S19" s="9">
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
-      <c r="S19" s="9">
-        <f t="shared" si="5"/>
+      <c r="T19" s="9">
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
-      <c r="T19" s="9">
-        <f t="shared" si="5"/>
+      <c r="U19" s="9">
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
-      <c r="U19" s="9">
-        <f t="shared" si="5"/>
+      <c r="V19" s="9">
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Death Knight Blood on going
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5606C801-8B27-4D79-BCC8-C2C011BF6B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6FA7C3-0A27-4766-B161-D84FBA149D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Warrior</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Death Knight_Plague</t>
+  </si>
+  <si>
+    <t>Death Knight_Blood</t>
   </si>
 </sst>
 </file>
@@ -2138,19 +2141,19 @@
         <v>105</v>
       </c>
       <c r="J8" s="7">
-        <f>'Property List'!S4</f>
-        <v>75</v>
-      </c>
-      <c r="K8" s="7">
         <f>'Property List'!T4</f>
         <v>75</v>
       </c>
-      <c r="L8" s="7">
+      <c r="K8" s="7">
         <f>'Property List'!U4</f>
         <v>75</v>
       </c>
+      <c r="L8" s="7">
+        <f>'Property List'!V4</f>
+        <v>75</v>
+      </c>
       <c r="M8" s="7">
-        <f>'Property List'!V4</f>
+        <f>'Property List'!W4</f>
         <v>75</v>
       </c>
       <c r="N8" s="4">
@@ -2206,19 +2209,19 @@
         <v>65</v>
       </c>
       <c r="J9" s="7">
-        <f>'Property List'!S7</f>
-        <v>75</v>
-      </c>
-      <c r="K9" s="7">
         <f>'Property List'!T7</f>
         <v>75</v>
       </c>
-      <c r="L9" s="7">
+      <c r="K9" s="7">
         <f>'Property List'!U7</f>
         <v>75</v>
       </c>
+      <c r="L9" s="7">
+        <f>'Property List'!V7</f>
+        <v>75</v>
+      </c>
       <c r="M9" s="7">
-        <f>'Property List'!V7</f>
+        <f>'Property List'!W7</f>
         <v>75</v>
       </c>
       <c r="N9" s="4">
@@ -2274,19 +2277,19 @@
         <v>50</v>
       </c>
       <c r="J10" s="7">
-        <f>'Property List'!S10</f>
-        <v>27</v>
-      </c>
-      <c r="K10" s="7">
         <f>'Property List'!T10</f>
         <v>27</v>
       </c>
-      <c r="L10" s="7">
+      <c r="K10" s="7">
         <f>'Property List'!U10</f>
         <v>27</v>
       </c>
+      <c r="L10" s="7">
+        <f>'Property List'!V10</f>
+        <v>27</v>
+      </c>
       <c r="M10" s="7">
-        <f>'Property List'!V10</f>
+        <f>'Property List'!W10</f>
         <v>27</v>
       </c>
       <c r="N10" s="4">
@@ -2342,19 +2345,19 @@
         <v>15</v>
       </c>
       <c r="J11" s="7">
-        <f>'Property List'!S13</f>
-        <v>25</v>
-      </c>
-      <c r="K11" s="7">
         <f>'Property List'!T13</f>
         <v>25</v>
       </c>
-      <c r="L11" s="7">
+      <c r="K11" s="7">
         <f>'Property List'!U13</f>
         <v>25</v>
       </c>
+      <c r="L11" s="7">
+        <f>'Property List'!V13</f>
+        <v>25</v>
+      </c>
       <c r="M11" s="7">
-        <f>'Property List'!V13</f>
+        <f>'Property List'!W13</f>
         <v>25</v>
       </c>
       <c r="N11" s="4">
@@ -2410,19 +2413,19 @@
         <v>31</v>
       </c>
       <c r="J12" s="2">
-        <f>'Property List'!S17</f>
-        <v>34</v>
-      </c>
-      <c r="K12" s="2">
         <f>'Property List'!T17</f>
         <v>34</v>
       </c>
-      <c r="L12" s="2">
+      <c r="K12" s="2">
         <f>'Property List'!U17</f>
         <v>34</v>
       </c>
+      <c r="L12" s="2">
+        <f>'Property List'!V17</f>
+        <v>34</v>
+      </c>
       <c r="M12" s="2">
-        <f>'Property List'!V17</f>
+        <f>'Property List'!W17</f>
         <v>34</v>
       </c>
       <c r="N12" s="4">
@@ -29892,13 +29895,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29916,10 +29919,10 @@
     <col min="15" max="15" width="16.21875" customWidth="1"/>
     <col min="16" max="16" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>17</v>
@@ -29973,19 +29976,22 @@
         <v>45</v>
       </c>
       <c r="S1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
@@ -30040,8 +30046,8 @@
       <c r="R2" s="9">
         <v>110</v>
       </c>
-      <c r="S2" s="2">
-        <v>80</v>
+      <c r="S2" s="9">
+        <v>110</v>
       </c>
       <c r="T2" s="2">
         <v>80</v>
@@ -30052,8 +30058,11 @@
       <c r="V2" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W2" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>33</v>
       </c>
@@ -30108,8 +30117,8 @@
       <c r="R3" s="9">
         <v>100</v>
       </c>
-      <c r="S3" s="2">
-        <v>70</v>
+      <c r="S3" s="9">
+        <v>100</v>
       </c>
       <c r="T3" s="2">
         <v>70</v>
@@ -30120,13 +30129,16 @@
       <c r="V3" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W3" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:V4" si="0">(B2+B3)/2</f>
+        <f t="shared" ref="B4:W4" si="0">(B2+B3)/2</f>
         <v>100</v>
       </c>
       <c r="C4" s="2">
@@ -30190,12 +30202,12 @@
         <v>105</v>
       </c>
       <c r="R4" s="2">
-        <f t="shared" ref="R4" si="1">(R2+R3)/2</f>
+        <f t="shared" ref="R4:S4" si="1">(R2+R3)/2</f>
         <v>105</v>
       </c>
       <c r="S4" s="2">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f t="shared" si="1"/>
+        <v>105</v>
       </c>
       <c r="T4" s="2">
         <f t="shared" si="0"/>
@@ -30209,8 +30221,12 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W4" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
@@ -30265,8 +30281,8 @@
       <c r="R5" s="9">
         <v>70</v>
       </c>
-      <c r="S5" s="2">
-        <v>80</v>
+      <c r="S5" s="9">
+        <v>70</v>
       </c>
       <c r="T5" s="2">
         <v>80</v>
@@ -30277,8 +30293,11 @@
       <c r="V5" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W5" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
@@ -30334,7 +30353,7 @@
         <v>60</v>
       </c>
       <c r="S6" s="9">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="T6" s="9">
         <v>70</v>
@@ -30345,13 +30364,16 @@
       <c r="V6" s="9">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W6" s="9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="9">
-        <f t="shared" ref="B7:V7" si="2">(B5+B6)/2</f>
+        <f t="shared" ref="B7:W7" si="2">(B5+B6)/2</f>
         <v>70</v>
       </c>
       <c r="C7" s="9">
@@ -30415,12 +30437,12 @@
         <v>65</v>
       </c>
       <c r="R7" s="9">
-        <f t="shared" ref="R7" si="3">(R5+R6)/2</f>
+        <f t="shared" ref="R7:S7" si="3">(R5+R6)/2</f>
         <v>65</v>
       </c>
       <c r="S7" s="9">
-        <f t="shared" si="2"/>
-        <v>75</v>
+        <f t="shared" si="3"/>
+        <v>65</v>
       </c>
       <c r="T7" s="9">
         <f t="shared" si="2"/>
@@ -30434,8 +30456,12 @@
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W7" s="9">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
@@ -30491,7 +30517,7 @@
         <v>55</v>
       </c>
       <c r="S8" s="9">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="T8" s="9">
         <v>30</v>
@@ -30502,8 +30528,11 @@
       <c r="V8" s="9">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W8" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
@@ -30559,7 +30588,7 @@
         <v>45</v>
       </c>
       <c r="S9" s="9">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="T9" s="9">
         <v>24</v>
@@ -30570,13 +30599,16 @@
       <c r="V9" s="9">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W9" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <f t="shared" ref="B10:V10" si="4">(B8+B9)/2</f>
+        <f t="shared" ref="B10:W10" si="4">(B8+B9)/2</f>
         <v>55</v>
       </c>
       <c r="C10" s="9">
@@ -30640,12 +30672,12 @@
         <v>50</v>
       </c>
       <c r="R10" s="9">
-        <f t="shared" ref="R10" si="5">(R8+R9)/2</f>
+        <f t="shared" ref="R10:S10" si="5">(R8+R9)/2</f>
         <v>50</v>
       </c>
       <c r="S10" s="9">
-        <f t="shared" si="4"/>
-        <v>27</v>
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="T10" s="9">
         <f t="shared" si="4"/>
@@ -30659,8 +30691,12 @@
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W10" s="9">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>38</v>
       </c>
@@ -30716,7 +30752,7 @@
         <v>20</v>
       </c>
       <c r="S11" s="9">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T11" s="9">
         <v>30</v>
@@ -30727,8 +30763,11 @@
       <c r="V11" s="9">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W11" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
@@ -30784,7 +30823,7 @@
         <v>10</v>
       </c>
       <c r="S12" s="9">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="T12" s="9">
         <v>20</v>
@@ -30795,13 +30834,16 @@
       <c r="V12" s="9">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W12" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="9">
-        <f t="shared" ref="B13:V13" si="6">(B11+B12)/2</f>
+        <f t="shared" ref="B13:W13" si="6">(B11+B12)/2</f>
         <v>15</v>
       </c>
       <c r="C13" s="9">
@@ -30865,12 +30907,12 @@
         <v>15</v>
       </c>
       <c r="R13" s="9">
-        <f t="shared" ref="R13" si="7">(R11+R12)/2</f>
+        <f t="shared" ref="R13:S13" si="7">(R11+R12)/2</f>
         <v>15</v>
       </c>
       <c r="S13" s="9">
-        <f t="shared" si="6"/>
-        <v>25</v>
+        <f t="shared" si="7"/>
+        <v>15</v>
       </c>
       <c r="T13" s="9">
         <f t="shared" si="6"/>
@@ -30884,8 +30926,12 @@
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W13" s="9">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>40</v>
       </c>
@@ -30952,8 +30998,11 @@
       <c r="V14" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W14" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>41</v>
       </c>
@@ -31020,13 +31069,16 @@
       <c r="V15" s="9">
         <v>-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W15" s="9">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="9">
-        <f t="shared" ref="B16:V16" si="8">(B14+B15)/2</f>
+        <f t="shared" ref="B16:W16" si="8">(B14+B15)/2</f>
         <v>0</v>
       </c>
       <c r="C16" s="9">
@@ -31090,11 +31142,11 @@
         <v>0</v>
       </c>
       <c r="R16" s="9">
-        <f t="shared" ref="R16" si="9">(R14+R15)/2</f>
+        <f t="shared" ref="R16:S16" si="9">(R14+R15)/2</f>
         <v>0</v>
       </c>
       <c r="S16" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T16" s="9">
@@ -31109,8 +31161,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W16" s="9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
@@ -31166,7 +31222,7 @@
         <v>31</v>
       </c>
       <c r="S17" s="9">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="T17" s="9">
         <v>34</v>
@@ -31177,8 +31233,11 @@
       <c r="V17" s="9">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="W17" s="9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -31201,13 +31260,14 @@
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
-    </row>
-    <row r="19" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="W18" s="9"/>
+    </row>
+    <row r="19" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="9">
-        <f t="shared" ref="B19:V19" si="10">B4+B7+B10+B13+B16+B17</f>
+        <f t="shared" ref="B19:W19" si="10">B4+B7+B10+B13+B16+B17</f>
         <v>265</v>
       </c>
       <c r="C19" s="9">
@@ -31271,12 +31331,12 @@
         <v>266</v>
       </c>
       <c r="R19" s="9">
-        <f t="shared" ref="R19" si="11">R4+R7+R10+R13+R16+R17</f>
+        <f t="shared" ref="R19:S19" si="11">R4+R7+R10+R13+R16+R17</f>
         <v>266</v>
       </c>
       <c r="S19" s="9">
-        <f t="shared" si="10"/>
-        <v>236</v>
+        <f t="shared" si="11"/>
+        <v>266</v>
       </c>
       <c r="T19" s="9">
         <f t="shared" si="10"/>
@@ -31287,6 +31347,10 @@
         <v>236</v>
       </c>
       <c r="V19" s="9">
+        <f t="shared" si="10"/>
+        <v>236</v>
+      </c>
+      <c r="W19" s="9">
         <f t="shared" si="10"/>
         <v>236</v>
       </c>

</xml_diff>

<commit_message>
Add Rogue Toxicology property
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856B8354-BE6D-44AC-9BC9-CF6ED46E1ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9C8A3B-588B-42C3-8959-D4B52418E6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>Rogue_Comprehensiveness</t>
   </si>
   <si>
-    <t>Mage_Comprehensiveness</t>
-  </si>
-  <si>
     <t>Priest_Comprehensiveness</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>Rogue_Assassination</t>
+  </si>
+  <si>
+    <t>Rogue_Toxicology</t>
   </si>
 </sst>
 </file>
@@ -935,19 +935,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.68181818181818177</c:v>
+                  <c:v>0.72727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9375</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49090909090909091</c:v>
+                  <c:v>0.67272727272727273</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.625</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.91891891891891897</c:v>
+                  <c:v>0.64864864864864868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="E2" s="11">
         <f t="shared" si="0"/>
-        <v>0.68181818181818177</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="F2" s="11">
         <f t="shared" si="0"/>
@@ -3014,7 +3014,7 @@
       </c>
       <c r="E3" s="12">
         <f t="shared" si="1"/>
-        <v>0.9375</v>
+        <v>1</v>
       </c>
       <c r="F3" s="12">
         <f t="shared" si="1"/>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="E4" s="12">
         <f t="shared" si="2"/>
-        <v>0.49090909090909091</v>
+        <v>0.67272727272727273</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" si="2"/>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="E5" s="12">
         <f t="shared" si="3"/>
-        <v>0.625</v>
+        <v>1</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="3"/>
@@ -3212,7 +3212,7 @@
       </c>
       <c r="E6" s="18">
         <f t="shared" si="4"/>
-        <v>0.91891891891891897</v>
+        <v>0.64864864864864868</v>
       </c>
       <c r="F6" s="18">
         <f t="shared" si="4"/>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="E8" s="22">
         <f>'Property List'!J4</f>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F8" s="23">
         <f>'Property List'!K4</f>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="E9" s="22">
         <f>'Property List'!J7</f>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F9" s="23">
         <f>'Property List'!K7</f>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="E10" s="22">
         <f>'Property List'!J10</f>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F10" s="23">
         <f>'Property List'!K10</f>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="E11" s="22">
         <f>'Property List'!J13</f>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F11" s="23">
         <f>'Property List'!K13</f>
@@ -3578,7 +3578,7 @@
       </c>
       <c r="E12" s="22">
         <f>'Property List'!J17</f>
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F12" s="22">
         <f>'Property List'!K17</f>
@@ -31083,7 +31083,7 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31094,8 +31094,7 @@
     <col min="4" max="4" width="26.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
     <col min="6" max="8" width="26" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26.33203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="30.88671875" style="1" customWidth="1"/>
     <col min="11" max="11" width="27.44140625" style="1" customWidth="1"/>
     <col min="12" max="16" width="31" style="1" customWidth="1"/>
     <col min="17" max="17" width="26.21875" style="1" customWidth="1"/>
@@ -31131,46 +31130,46 @@
         <v>23</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="W1" s="29" t="s">
         <v>8</v>
@@ -31187,7 +31186,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="22">
         <v>105</v>
@@ -31214,7 +31213,7 @@
         <v>85</v>
       </c>
       <c r="J2" s="22">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="K2" s="23">
         <v>95</v>
@@ -31267,7 +31266,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="22">
         <v>95</v>
@@ -31294,7 +31293,7 @@
         <v>75</v>
       </c>
       <c r="J3" s="22">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="K3" s="23">
         <v>85</v>
@@ -31382,8 +31381,8 @@
         <v>80</v>
       </c>
       <c r="J4" s="22">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f t="shared" ref="J4" si="1">(J2+J3)/2</f>
+        <v>80</v>
       </c>
       <c r="K4" s="22">
         <f t="shared" si="0"/>
@@ -31452,7 +31451,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="22">
         <v>75</v>
@@ -31479,7 +31478,7 @@
         <v>85</v>
       </c>
       <c r="J5" s="22">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="K5" s="23">
         <v>65</v>
@@ -31532,7 +31531,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="39">
         <v>65</v>
@@ -31559,7 +31558,7 @@
         <v>75</v>
       </c>
       <c r="J6" s="40">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="K6" s="40">
         <v>55</v>
@@ -31615,109 +31614,109 @@
         <v>13</v>
       </c>
       <c r="B7" s="31">
-        <f t="shared" ref="B7:Z7" si="1">(B5+B6)/2</f>
+        <f t="shared" ref="B7:Z7" si="2">(B5+B6)/2</f>
         <v>70</v>
       </c>
       <c r="C7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="D7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="E7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="F7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="G7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="H7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="I7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="J7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J7" si="3">(J5+J6)/2</f>
+        <v>80</v>
+      </c>
+      <c r="K7" s="32">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="L7" s="32">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="M7" s="32">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="N7" s="32">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="O7" s="32">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="P7" s="32">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="Q7" s="32">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="R7" s="32">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="S7" s="32">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="T7" s="32">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="U7" s="32">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="V7" s="32">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="W7" s="32">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="K7" s="32">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="L7" s="32">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="M7" s="32">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="N7" s="32">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="O7" s="32">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="P7" s="32">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="Q7" s="32">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="R7" s="32">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="S7" s="32">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="T7" s="32">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="U7" s="32">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="V7" s="32">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="W7" s="32">
-        <f t="shared" si="1"/>
+      <c r="X7" s="32">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="X7" s="32">
-        <f t="shared" si="1"/>
+      <c r="Y7" s="32">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="Y7" s="32">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
       <c r="Z7" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="31">
         <v>60</v>
@@ -31744,7 +31743,7 @@
         <v>40</v>
       </c>
       <c r="J8" s="32">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K8" s="32">
         <v>40</v>
@@ -31797,7 +31796,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="31">
         <v>50</v>
@@ -31824,7 +31823,7 @@
         <v>34</v>
       </c>
       <c r="J9" s="32">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="K9" s="32">
         <v>34</v>
@@ -31880,109 +31879,109 @@
         <v>14</v>
       </c>
       <c r="B10" s="31">
-        <f t="shared" ref="B10:Z10" si="2">(B8+B9)/2</f>
+        <f t="shared" ref="B10:Z10" si="4">(B8+B9)/2</f>
         <v>55</v>
       </c>
       <c r="C10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="D10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="E10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="F10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="G10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="H10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="I10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="J10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J10" si="5">(J8+J9)/2</f>
+        <v>37</v>
+      </c>
+      <c r="K10" s="32">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="L10" s="32">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="M10" s="32">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="N10" s="32">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="O10" s="32">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="P10" s="32">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="Q10" s="32">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="K10" s="32">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="L10" s="32">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="M10" s="32">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="N10" s="32">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="O10" s="32">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="P10" s="32">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="Q10" s="32">
-        <f t="shared" si="2"/>
+      <c r="R10" s="32">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="R10" s="32">
-        <f t="shared" si="2"/>
+      <c r="S10" s="32">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="S10" s="32">
-        <f t="shared" si="2"/>
+      <c r="T10" s="32">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="U10" s="32">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="V10" s="32">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="W10" s="32">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="T10" s="32">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="U10" s="32">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="V10" s="32">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="W10" s="32">
-        <f t="shared" si="2"/>
+      <c r="X10" s="32">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="X10" s="32">
-        <f t="shared" si="2"/>
+      <c r="Y10" s="32">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="Y10" s="32">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
       <c r="Z10" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="31">
         <v>20</v>
@@ -32009,7 +32008,7 @@
         <v>45</v>
       </c>
       <c r="J11" s="32">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="K11" s="32">
         <v>25</v>
@@ -32062,7 +32061,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="31">
         <v>10</v>
@@ -32089,7 +32088,7 @@
         <v>35</v>
       </c>
       <c r="J12" s="32">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="K12" s="32">
         <v>15</v>
@@ -32145,109 +32144,109 @@
         <v>15</v>
       </c>
       <c r="B13" s="31">
-        <f t="shared" ref="B13:Z13" si="3">(B11+B12)/2</f>
+        <f t="shared" ref="B13:Z13" si="6">(B11+B12)/2</f>
         <v>15</v>
       </c>
       <c r="C13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="D13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="E13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="F13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="G13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="H13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="I13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="J13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J13" si="7">(J11+J12)/2</f>
+        <v>40</v>
+      </c>
+      <c r="K13" s="32">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="L13" s="32">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="M13" s="32">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="N13" s="32">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="O13" s="32">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="P13" s="32">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="Q13" s="32">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="K13" s="32">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="L13" s="32">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="M13" s="32">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="N13" s="32">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="O13" s="32">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="P13" s="32">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="Q13" s="32">
-        <f t="shared" si="3"/>
+      <c r="R13" s="32">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="R13" s="32">
-        <f t="shared" si="3"/>
+      <c r="S13" s="32">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="S13" s="32">
-        <f t="shared" si="3"/>
+      <c r="T13" s="32">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="U13" s="32">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="V13" s="32">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="W13" s="32">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="T13" s="32">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="U13" s="32">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="V13" s="32">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="W13" s="32">
-        <f t="shared" si="3"/>
+      <c r="X13" s="32">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="X13" s="32">
-        <f t="shared" si="3"/>
+      <c r="Y13" s="32">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="Y13" s="32">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
       <c r="Z13" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="31">
         <v>5</v>
@@ -32327,7 +32326,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="31">
         <v>-5</v>
@@ -32407,106 +32406,106 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="31">
-        <f t="shared" ref="B16:Z16" si="4">(B14+B15)/2</f>
+        <f t="shared" ref="B16:Z16" si="8">(B14+B15)/2</f>
         <v>0</v>
       </c>
       <c r="C16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J16" si="9">(J14+J15)/2</f>
         <v>0</v>
       </c>
       <c r="K16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -32539,7 +32538,7 @@
         <v>24</v>
       </c>
       <c r="J17" s="32">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K17" s="32">
         <v>37</v>
@@ -32620,106 +32619,106 @@
     </row>
     <row r="19" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="32">
-        <f t="shared" ref="B19:Z19" si="5">B4+B7+B10+B13+B16+B17</f>
+        <f t="shared" ref="B19:Z19" si="10">B4+B7+B10+B13+B16+B17</f>
         <v>265</v>
       </c>
       <c r="C19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>204</v>
       </c>
       <c r="D19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>199</v>
       </c>
       <c r="E19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>266</v>
       </c>
       <c r="F19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>266</v>
       </c>
       <c r="G19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>266</v>
       </c>
       <c r="H19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>261</v>
       </c>
       <c r="I19" s="32">
-        <f t="shared" ref="I19" si="6">I4+I7+I10+I13+I16+I17</f>
+        <f t="shared" ref="I19:J19" si="11">I4+I7+I10+I13+I16+I17</f>
         <v>261</v>
       </c>
       <c r="J19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
+        <v>261</v>
+      </c>
+      <c r="K19" s="32">
+        <f t="shared" si="10"/>
+        <v>244</v>
+      </c>
+      <c r="L19" s="32">
+        <f t="shared" si="10"/>
+        <v>244</v>
+      </c>
+      <c r="M19" s="32">
+        <f t="shared" si="10"/>
+        <v>244</v>
+      </c>
+      <c r="N19" s="32">
+        <f t="shared" si="10"/>
+        <v>244</v>
+      </c>
+      <c r="O19" s="32">
+        <f t="shared" si="10"/>
+        <v>244</v>
+      </c>
+      <c r="P19" s="32">
+        <f t="shared" si="10"/>
+        <v>246</v>
+      </c>
+      <c r="Q19" s="32">
+        <f t="shared" si="10"/>
+        <v>251</v>
+      </c>
+      <c r="R19" s="32">
+        <f t="shared" si="10"/>
+        <v>251</v>
+      </c>
+      <c r="S19" s="32">
+        <f t="shared" si="10"/>
+        <v>251</v>
+      </c>
+      <c r="T19" s="32">
+        <f t="shared" si="10"/>
+        <v>266</v>
+      </c>
+      <c r="U19" s="32">
+        <f t="shared" si="10"/>
+        <v>266</v>
+      </c>
+      <c r="V19" s="32">
+        <f t="shared" si="10"/>
+        <v>266</v>
+      </c>
+      <c r="W19" s="32">
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
-      <c r="K19" s="32">
-        <f t="shared" si="5"/>
-        <v>244</v>
-      </c>
-      <c r="L19" s="32">
-        <f t="shared" si="5"/>
-        <v>244</v>
-      </c>
-      <c r="M19" s="32">
-        <f t="shared" si="5"/>
-        <v>244</v>
-      </c>
-      <c r="N19" s="32">
-        <f t="shared" si="5"/>
-        <v>244</v>
-      </c>
-      <c r="O19" s="32">
-        <f t="shared" si="5"/>
-        <v>244</v>
-      </c>
-      <c r="P19" s="32">
-        <f t="shared" si="5"/>
-        <v>246</v>
-      </c>
-      <c r="Q19" s="32">
-        <f t="shared" si="5"/>
-        <v>251</v>
-      </c>
-      <c r="R19" s="32">
-        <f t="shared" si="5"/>
-        <v>251</v>
-      </c>
-      <c r="S19" s="32">
-        <f t="shared" si="5"/>
-        <v>251</v>
-      </c>
-      <c r="T19" s="32">
-        <f t="shared" si="5"/>
-        <v>266</v>
-      </c>
-      <c r="U19" s="32">
-        <f t="shared" si="5"/>
-        <v>266</v>
-      </c>
-      <c r="V19" s="32">
-        <f t="shared" si="5"/>
-        <v>266</v>
-      </c>
-      <c r="W19" s="32">
-        <f t="shared" si="5"/>
+      <c r="X19" s="32">
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
-      <c r="X19" s="32">
-        <f t="shared" si="5"/>
+      <c r="Y19" s="32">
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
-      <c r="Y19" s="32">
-        <f t="shared" si="5"/>
-        <v>236</v>
-      </c>
       <c r="Z19" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Water Elemental and Mage Water
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731FD7FA-2158-4650-A718-0567426FAFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67E74E0-1101-4227-AC41-2CAFF7CDED0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14625" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bar" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>Warrior</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Mage_Comprehensiveness</t>
+  </si>
+  <si>
+    <t>Warrior_Water_Elemental</t>
   </si>
 </sst>
 </file>
@@ -3300,47 +3303,47 @@
         <v>100</v>
       </c>
       <c r="C8" s="22">
-        <f>'Property List'!E4</f>
+        <f>'Property List'!F4</f>
         <v>110</v>
       </c>
       <c r="D8" s="22">
-        <f>'Property List'!H4</f>
+        <f>'Property List'!I4</f>
         <v>80</v>
       </c>
       <c r="E8" s="22">
-        <f>'Property List'!J4</f>
+        <f>'Property List'!K4</f>
         <v>80</v>
       </c>
       <c r="F8" s="23">
-        <f>'Property List'!K4</f>
+        <f>'Property List'!L4</f>
         <v>90</v>
       </c>
       <c r="G8" s="23">
-        <f>'Property List'!P4</f>
+        <f>'Property List'!Q4</f>
         <v>85</v>
       </c>
       <c r="H8" s="23">
-        <f>'Property List'!Q4</f>
+        <f>'Property List'!R4</f>
         <v>95</v>
       </c>
       <c r="I8" s="23">
-        <f>'Property List'!T4</f>
+        <f>'Property List'!U4</f>
         <v>105</v>
       </c>
       <c r="J8" s="23">
-        <f>'Property List'!W4</f>
-        <v>75</v>
-      </c>
-      <c r="K8" s="23">
         <f>'Property List'!X4</f>
         <v>75</v>
       </c>
-      <c r="L8" s="23">
+      <c r="K8" s="23">
         <f>'Property List'!Y4</f>
         <v>75</v>
       </c>
+      <c r="L8" s="23">
+        <f>'Property List'!Z4</f>
+        <v>75</v>
+      </c>
       <c r="M8" s="23">
-        <f>'Property List'!Z4</f>
+        <f>'Property List'!AA4</f>
         <v>75</v>
       </c>
       <c r="N8" s="24">
@@ -3368,47 +3371,47 @@
         <v>70</v>
       </c>
       <c r="C9" s="22">
-        <f>'Property List'!E7</f>
+        <f>'Property List'!F7</f>
         <v>70</v>
       </c>
       <c r="D9" s="22">
-        <f>'Property List'!H7</f>
+        <f>'Property List'!I7</f>
         <v>80</v>
       </c>
       <c r="E9" s="22">
-        <f>'Property List'!J7</f>
+        <f>'Property List'!K7</f>
         <v>80</v>
       </c>
       <c r="F9" s="23">
-        <f>'Property List'!K7</f>
+        <f>'Property List'!L7</f>
         <v>60</v>
       </c>
       <c r="G9" s="23">
-        <f>'Property List'!P7</f>
+        <f>'Property List'!Q7</f>
         <v>65</v>
       </c>
       <c r="H9" s="23">
-        <f>'Property List'!Q7</f>
+        <f>'Property List'!R7</f>
         <v>70</v>
       </c>
       <c r="I9" s="23">
-        <f>'Property List'!T7</f>
+        <f>'Property List'!U7</f>
         <v>65</v>
       </c>
       <c r="J9" s="23">
-        <f>'Property List'!W7</f>
-        <v>75</v>
-      </c>
-      <c r="K9" s="23">
         <f>'Property List'!X7</f>
         <v>75</v>
       </c>
-      <c r="L9" s="23">
+      <c r="K9" s="23">
         <f>'Property List'!Y7</f>
         <v>75</v>
       </c>
+      <c r="L9" s="23">
+        <f>'Property List'!Z7</f>
+        <v>75</v>
+      </c>
       <c r="M9" s="23">
-        <f>'Property List'!Z7</f>
+        <f>'Property List'!AA7</f>
         <v>75</v>
       </c>
       <c r="N9" s="24">
@@ -3436,47 +3439,47 @@
         <v>55</v>
       </c>
       <c r="C10" s="22">
-        <f>'Property List'!E10</f>
+        <f>'Property List'!F10</f>
         <v>45</v>
       </c>
       <c r="D10" s="22">
-        <f>'Property List'!H10</f>
+        <f>'Property List'!I10</f>
         <v>37</v>
       </c>
       <c r="E10" s="22">
-        <f>'Property List'!J10</f>
-        <v>37</v>
-      </c>
-      <c r="F10" s="23">
         <f>'Property List'!K10</f>
         <v>37</v>
       </c>
+      <c r="F10" s="23">
+        <f>'Property List'!L10</f>
+        <v>37</v>
+      </c>
       <c r="G10" s="23">
-        <f>'Property List'!P10</f>
+        <f>'Property List'!Q10</f>
         <v>32</v>
       </c>
       <c r="H10" s="23">
-        <f>'Property List'!Q10</f>
+        <f>'Property List'!R10</f>
         <v>27</v>
       </c>
       <c r="I10" s="23">
-        <f>'Property List'!T10</f>
+        <f>'Property List'!U10</f>
         <v>50</v>
       </c>
       <c r="J10" s="23">
-        <f>'Property List'!W10</f>
-        <v>27</v>
-      </c>
-      <c r="K10" s="23">
         <f>'Property List'!X10</f>
         <v>27</v>
       </c>
-      <c r="L10" s="23">
+      <c r="K10" s="23">
         <f>'Property List'!Y10</f>
         <v>27</v>
       </c>
+      <c r="L10" s="23">
+        <f>'Property List'!Z10</f>
+        <v>27</v>
+      </c>
       <c r="M10" s="23">
-        <f>'Property List'!Z10</f>
+        <f>'Property List'!AA10</f>
         <v>27</v>
       </c>
       <c r="N10" s="24">
@@ -3504,47 +3507,47 @@
         <v>15</v>
       </c>
       <c r="C11" s="22">
-        <f>'Property List'!E13</f>
+        <f>'Property List'!F13</f>
         <v>10</v>
       </c>
       <c r="D11" s="22">
-        <f>'Property List'!H13</f>
+        <f>'Property List'!I13</f>
         <v>40</v>
       </c>
       <c r="E11" s="22">
-        <f>'Property List'!J13</f>
+        <f>'Property List'!K13</f>
         <v>40</v>
       </c>
       <c r="F11" s="23">
-        <f>'Property List'!K13</f>
+        <f>'Property List'!L13</f>
         <v>20</v>
       </c>
       <c r="G11" s="23">
-        <f>'Property List'!P13</f>
+        <f>'Property List'!Q13</f>
         <v>30</v>
       </c>
       <c r="H11" s="23">
-        <f>'Property List'!Q13</f>
+        <f>'Property List'!R13</f>
         <v>25</v>
       </c>
       <c r="I11" s="23">
-        <f>'Property List'!T13</f>
+        <f>'Property List'!U13</f>
         <v>15</v>
       </c>
       <c r="J11" s="23">
-        <f>'Property List'!W13</f>
-        <v>25</v>
-      </c>
-      <c r="K11" s="23">
         <f>'Property List'!X13</f>
         <v>25</v>
       </c>
-      <c r="L11" s="23">
+      <c r="K11" s="23">
         <f>'Property List'!Y13</f>
         <v>25</v>
       </c>
+      <c r="L11" s="23">
+        <f>'Property List'!Z13</f>
+        <v>25</v>
+      </c>
       <c r="M11" s="23">
-        <f>'Property List'!Z13</f>
+        <f>'Property List'!AA13</f>
         <v>25</v>
       </c>
       <c r="N11" s="24">
@@ -3572,47 +3575,47 @@
         <v>25</v>
       </c>
       <c r="C12" s="22">
-        <f>'Property List'!E17</f>
+        <f>'Property List'!F17</f>
         <v>31</v>
       </c>
       <c r="D12" s="22">
-        <f>'Property List'!H17</f>
+        <f>'Property List'!I17</f>
         <v>24</v>
       </c>
       <c r="E12" s="22">
-        <f>'Property List'!J17</f>
+        <f>'Property List'!K17</f>
         <v>24</v>
       </c>
       <c r="F12" s="22">
-        <f>'Property List'!K17</f>
+        <f>'Property List'!L17</f>
         <v>37</v>
       </c>
       <c r="G12" s="22">
-        <f>'Property List'!P17</f>
-        <v>34</v>
-      </c>
-      <c r="H12" s="22">
         <f>'Property List'!Q17</f>
         <v>34</v>
       </c>
+      <c r="H12" s="22">
+        <f>'Property List'!R17</f>
+        <v>34</v>
+      </c>
       <c r="I12" s="22">
-        <f>'Property List'!T17</f>
+        <f>'Property List'!U17</f>
         <v>31</v>
       </c>
       <c r="J12" s="22">
-        <f>'Property List'!W17</f>
-        <v>34</v>
-      </c>
-      <c r="K12" s="22">
         <f>'Property List'!X17</f>
         <v>34</v>
       </c>
-      <c r="L12" s="22">
+      <c r="K12" s="22">
         <f>'Property List'!Y17</f>
         <v>34</v>
       </c>
+      <c r="L12" s="22">
+        <f>'Property List'!Z17</f>
+        <v>34</v>
+      </c>
       <c r="M12" s="22">
-        <f>'Property List'!Z17</f>
+        <f>'Property List'!AA17</f>
         <v>34</v>
       </c>
       <c r="N12" s="24">
@@ -31083,34 +31086,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="8" width="26" style="1" customWidth="1"/>
-    <col min="9" max="10" width="30.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27.44140625" style="1" customWidth="1"/>
-    <col min="12" max="16" width="31" style="1" customWidth="1"/>
-    <col min="17" max="17" width="26.21875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16.21875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="19.44140625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="18.21875" style="1" customWidth="1"/>
-    <col min="21" max="22" width="19.6640625" style="1" customWidth="1"/>
-    <col min="23" max="26" width="12.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="12.6640625" style="1"/>
+    <col min="4" max="5" width="26.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32" style="1" customWidth="1"/>
+    <col min="7" max="9" width="26" style="1" customWidth="1"/>
+    <col min="10" max="11" width="30.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="27.44140625" style="1" customWidth="1"/>
+    <col min="13" max="17" width="31" style="1" customWidth="1"/>
+    <col min="18" max="18" width="26.21875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="19.44140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.21875" style="1" customWidth="1"/>
+    <col min="22" max="23" width="19.6640625" style="1" customWidth="1"/>
+    <col min="24" max="27" width="12.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>17</v>
@@ -31122,76 +31125,79 @@
         <v>19</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="X1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="Y1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="29" t="s">
+      <c r="Z1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="29" t="s">
+      <c r="AA1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="29" t="s">
+      <c r="AB1" s="29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>36</v>
       </c>
@@ -31205,16 +31211,16 @@
         <v>60</v>
       </c>
       <c r="E2" s="22">
+        <v>70</v>
+      </c>
+      <c r="F2" s="22">
         <v>115</v>
       </c>
-      <c r="F2" s="22">
+      <c r="G2" s="22">
         <v>120</v>
       </c>
-      <c r="G2" s="22">
+      <c r="H2" s="22">
         <v>115</v>
-      </c>
-      <c r="H2" s="22">
-        <v>85</v>
       </c>
       <c r="I2" s="22">
         <v>85</v>
@@ -31222,8 +31228,8 @@
       <c r="J2" s="22">
         <v>85</v>
       </c>
-      <c r="K2" s="23">
-        <v>95</v>
+      <c r="K2" s="22">
+        <v>85</v>
       </c>
       <c r="L2" s="23">
         <v>95</v>
@@ -31237,11 +31243,11 @@
       <c r="O2" s="23">
         <v>95</v>
       </c>
-      <c r="P2" s="31">
+      <c r="P2" s="23">
+        <v>95</v>
+      </c>
+      <c r="Q2" s="31">
         <v>90</v>
-      </c>
-      <c r="Q2" s="32">
-        <v>100</v>
       </c>
       <c r="R2" s="32">
         <v>100</v>
@@ -31250,16 +31256,16 @@
         <v>100</v>
       </c>
       <c r="T2" s="32">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="U2" s="32">
         <v>110</v>
       </c>
-      <c r="V2" s="33">
+      <c r="V2" s="32">
         <v>110</v>
       </c>
-      <c r="W2" s="22">
-        <v>80</v>
+      <c r="W2" s="33">
+        <v>110</v>
       </c>
       <c r="X2" s="22">
         <v>80</v>
@@ -31267,14 +31273,17 @@
       <c r="Y2" s="22">
         <v>80</v>
       </c>
-      <c r="Z2" s="34">
+      <c r="Z2" s="22">
         <v>80</v>
       </c>
       <c r="AA2" s="34">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB2" s="34">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>37</v>
       </c>
@@ -31288,16 +31297,16 @@
         <v>50</v>
       </c>
       <c r="E3" s="22">
+        <v>60</v>
+      </c>
+      <c r="F3" s="22">
         <v>105</v>
       </c>
-      <c r="F3" s="22">
+      <c r="G3" s="22">
         <v>110</v>
       </c>
-      <c r="G3" s="22">
+      <c r="H3" s="22">
         <v>105</v>
-      </c>
-      <c r="H3" s="22">
-        <v>75</v>
       </c>
       <c r="I3" s="22">
         <v>75</v>
@@ -31305,8 +31314,8 @@
       <c r="J3" s="22">
         <v>75</v>
       </c>
-      <c r="K3" s="23">
-        <v>85</v>
+      <c r="K3" s="22">
+        <v>75</v>
       </c>
       <c r="L3" s="23">
         <v>85</v>
@@ -31320,11 +31329,11 @@
       <c r="O3" s="23">
         <v>85</v>
       </c>
-      <c r="P3" s="36">
+      <c r="P3" s="23">
+        <v>85</v>
+      </c>
+      <c r="Q3" s="36">
         <v>80</v>
-      </c>
-      <c r="Q3" s="37">
-        <v>90</v>
       </c>
       <c r="R3" s="37">
         <v>90</v>
@@ -31333,16 +31342,16 @@
         <v>90</v>
       </c>
       <c r="T3" s="37">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="U3" s="37">
         <v>100</v>
       </c>
-      <c r="V3" s="38">
+      <c r="V3" s="37">
         <v>100</v>
       </c>
-      <c r="W3" s="22">
-        <v>70</v>
+      <c r="W3" s="38">
+        <v>100</v>
       </c>
       <c r="X3" s="22">
         <v>70</v>
@@ -31350,19 +31359,22 @@
       <c r="Y3" s="22">
         <v>70</v>
       </c>
-      <c r="Z3" s="34">
+      <c r="Z3" s="22">
         <v>70</v>
       </c>
       <c r="AA3" s="34">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB3" s="34">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="22">
-        <f t="shared" ref="B4:Z4" si="0">(B2+B3)/2</f>
+        <f t="shared" ref="B4:AA4" si="0">(B2+B3)/2</f>
         <v>100</v>
       </c>
       <c r="C4" s="22">
@@ -31374,32 +31386,32 @@
         <v>55</v>
       </c>
       <c r="E4" s="22">
+        <f t="shared" ref="E4" si="1">(E2+E3)/2</f>
+        <v>65</v>
+      </c>
+      <c r="F4" s="22">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="F4" s="22">
+      <c r="G4" s="22">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="G4" s="22">
+      <c r="H4" s="22">
         <f t="shared" si="0"/>
         <v>110</v>
-      </c>
-      <c r="H4" s="22">
-        <f t="shared" si="0"/>
-        <v>80</v>
       </c>
       <c r="I4" s="22">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="J4" s="22">
-        <f t="shared" ref="J4" si="1">(J2+J3)/2</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="K4" s="22">
-        <f t="shared" si="0"/>
-        <v>90</v>
+        <f t="shared" ref="K4" si="2">(K2+K3)/2</f>
+        <v>80</v>
       </c>
       <c r="L4" s="22">
         <f t="shared" si="0"/>
@@ -31419,11 +31431,11 @@
       </c>
       <c r="P4" s="22">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q4" s="22">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R4" s="22">
         <f t="shared" si="0"/>
@@ -31435,7 +31447,7 @@
       </c>
       <c r="T4" s="22">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="U4" s="22">
         <f t="shared" si="0"/>
@@ -31447,7 +31459,7 @@
       </c>
       <c r="W4" s="22">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="X4" s="22">
         <f t="shared" si="0"/>
@@ -31457,16 +31469,20 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="Z4" s="34">
+      <c r="Z4" s="22">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="AA4" s="34">
-        <f t="shared" ref="AA4" si="2">(AA2+AA3)/2</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB4" s="34">
+        <f t="shared" ref="AB4" si="3">(AB2+AB3)/2</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>38</v>
       </c>
@@ -31480,16 +31496,16 @@
         <v>70</v>
       </c>
       <c r="E5" s="22">
+        <v>65</v>
+      </c>
+      <c r="F5" s="22">
         <v>75</v>
       </c>
-      <c r="F5" s="22">
+      <c r="G5" s="22">
         <v>65</v>
       </c>
-      <c r="G5" s="22">
+      <c r="H5" s="22">
         <v>70</v>
-      </c>
-      <c r="H5" s="22">
-        <v>85</v>
       </c>
       <c r="I5" s="22">
         <v>85</v>
@@ -31497,8 +31513,8 @@
       <c r="J5" s="22">
         <v>85</v>
       </c>
-      <c r="K5" s="23">
-        <v>65</v>
+      <c r="K5" s="22">
+        <v>85</v>
       </c>
       <c r="L5" s="23">
         <v>65</v>
@@ -31512,11 +31528,11 @@
       <c r="O5" s="23">
         <v>65</v>
       </c>
-      <c r="P5" s="39">
+      <c r="P5" s="23">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="39">
         <v>70</v>
-      </c>
-      <c r="Q5" s="40">
-        <v>75</v>
       </c>
       <c r="R5" s="40">
         <v>75</v>
@@ -31525,16 +31541,16 @@
         <v>75</v>
       </c>
       <c r="T5" s="40">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="U5" s="40">
         <v>70</v>
       </c>
-      <c r="V5" s="41">
+      <c r="V5" s="40">
         <v>70</v>
       </c>
-      <c r="W5" s="22">
-        <v>80</v>
+      <c r="W5" s="41">
+        <v>70</v>
       </c>
       <c r="X5" s="22">
         <v>80</v>
@@ -31542,14 +31558,17 @@
       <c r="Y5" s="22">
         <v>80</v>
       </c>
-      <c r="Z5" s="34">
+      <c r="Z5" s="22">
         <v>80</v>
       </c>
       <c r="AA5" s="34">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB5" s="34">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>39</v>
       </c>
@@ -31563,16 +31582,16 @@
         <v>60</v>
       </c>
       <c r="E6" s="40">
+        <v>55</v>
+      </c>
+      <c r="F6" s="40">
         <v>65</v>
       </c>
-      <c r="F6" s="40">
+      <c r="G6" s="40">
         <v>55</v>
       </c>
-      <c r="G6" s="40">
+      <c r="H6" s="40">
         <v>60</v>
-      </c>
-      <c r="H6" s="40">
-        <v>75</v>
       </c>
       <c r="I6" s="40">
         <v>75</v>
@@ -31581,7 +31600,7 @@
         <v>75</v>
       </c>
       <c r="K6" s="40">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="L6" s="40">
         <v>55</v>
@@ -31595,11 +31614,11 @@
       <c r="O6" s="40">
         <v>55</v>
       </c>
-      <c r="P6" s="32">
+      <c r="P6" s="40">
+        <v>55</v>
+      </c>
+      <c r="Q6" s="32">
         <v>60</v>
-      </c>
-      <c r="Q6" s="32">
-        <v>65</v>
       </c>
       <c r="R6" s="32">
         <v>65</v>
@@ -31608,7 +31627,7 @@
         <v>65</v>
       </c>
       <c r="T6" s="32">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="U6" s="32">
         <v>60</v>
@@ -31616,8 +31635,8 @@
       <c r="V6" s="32">
         <v>60</v>
       </c>
-      <c r="W6" s="40">
-        <v>70</v>
+      <c r="W6" s="32">
+        <v>60</v>
       </c>
       <c r="X6" s="40">
         <v>70</v>
@@ -31631,117 +31650,124 @@
       <c r="AA6" s="40">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB6" s="40">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="31">
-        <f t="shared" ref="B7:Z7" si="3">(B5+B6)/2</f>
+        <f t="shared" ref="B7:AA7" si="4">(B5+B6)/2</f>
         <v>70</v>
       </c>
       <c r="C7" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="D7" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="E7" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E7" si="5">(E5+E6)/2</f>
+        <v>60</v>
+      </c>
+      <c r="F7" s="32">
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="F7" s="32">
-        <f t="shared" si="3"/>
+      <c r="G7" s="32">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="G7" s="32">
-        <f t="shared" si="3"/>
+      <c r="H7" s="32">
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="H7" s="32">
-        <f t="shared" si="3"/>
+      <c r="I7" s="32">
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="I7" s="32">
-        <f t="shared" si="3"/>
+      <c r="J7" s="32">
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="J7" s="32">
-        <f t="shared" ref="J7" si="4">(J5+J6)/2</f>
+      <c r="K7" s="32">
+        <f t="shared" ref="K7" si="6">(K5+K6)/2</f>
         <v>80</v>
       </c>
-      <c r="K7" s="32">
-        <f t="shared" si="3"/>
+      <c r="L7" s="32">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="L7" s="32">
-        <f t="shared" si="3"/>
+      <c r="M7" s="32">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="M7" s="32">
-        <f t="shared" si="3"/>
+      <c r="N7" s="32">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="N7" s="32">
-        <f t="shared" si="3"/>
+      <c r="O7" s="32">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="O7" s="32">
-        <f t="shared" si="3"/>
+      <c r="P7" s="32">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="P7" s="32">
-        <f t="shared" si="3"/>
+      <c r="Q7" s="32">
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="Q7" s="32">
-        <f t="shared" si="3"/>
+      <c r="R7" s="32">
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="R7" s="32">
-        <f t="shared" si="3"/>
+      <c r="S7" s="32">
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="S7" s="32">
-        <f t="shared" si="3"/>
+      <c r="T7" s="32">
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="T7" s="32">
-        <f t="shared" si="3"/>
+      <c r="U7" s="32">
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="U7" s="32">
-        <f t="shared" si="3"/>
+      <c r="V7" s="32">
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="V7" s="32">
-        <f t="shared" si="3"/>
+      <c r="W7" s="32">
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="W7" s="32">
-        <f t="shared" si="3"/>
+      <c r="X7" s="32">
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="X7" s="32">
-        <f t="shared" si="3"/>
+      <c r="Y7" s="32">
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="Y7" s="32">
-        <f t="shared" si="3"/>
+      <c r="Z7" s="32">
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="Z7" s="32">
-        <f t="shared" si="3"/>
+      <c r="AA7" s="32">
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="AA7" s="32">
-        <f t="shared" ref="AA7" si="5">(AA5+AA6)/2</f>
+      <c r="AB7" s="32">
+        <f t="shared" ref="AB7" si="7">(AB5+AB6)/2</f>
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>40</v>
       </c>
@@ -31755,16 +31781,16 @@
         <v>50</v>
       </c>
       <c r="E8" s="32">
+        <v>45</v>
+      </c>
+      <c r="F8" s="32">
         <v>50</v>
-      </c>
-      <c r="F8" s="32">
-        <v>55</v>
       </c>
       <c r="G8" s="32">
         <v>55</v>
       </c>
       <c r="H8" s="32">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="I8" s="32">
         <v>40</v>
@@ -31788,10 +31814,10 @@
         <v>40</v>
       </c>
       <c r="P8" s="32">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="32">
         <v>35</v>
-      </c>
-      <c r="Q8" s="32">
-        <v>30</v>
       </c>
       <c r="R8" s="32">
         <v>30</v>
@@ -31800,7 +31826,7 @@
         <v>30</v>
       </c>
       <c r="T8" s="32">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="U8" s="32">
         <v>55</v>
@@ -31809,7 +31835,7 @@
         <v>55</v>
       </c>
       <c r="W8" s="32">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="X8" s="32">
         <v>30</v>
@@ -31823,8 +31849,11 @@
       <c r="AA8" s="32">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB8" s="32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>41</v>
       </c>
@@ -31838,16 +31867,16 @@
         <v>40</v>
       </c>
       <c r="E9" s="32">
+        <v>35</v>
+      </c>
+      <c r="F9" s="32">
         <v>40</v>
-      </c>
-      <c r="F9" s="32">
-        <v>45</v>
       </c>
       <c r="G9" s="32">
         <v>45</v>
       </c>
       <c r="H9" s="32">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="I9" s="32">
         <v>34</v>
@@ -31871,10 +31900,10 @@
         <v>34</v>
       </c>
       <c r="P9" s="32">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="32">
         <v>29</v>
-      </c>
-      <c r="Q9" s="32">
-        <v>24</v>
       </c>
       <c r="R9" s="32">
         <v>24</v>
@@ -31883,7 +31912,7 @@
         <v>24</v>
       </c>
       <c r="T9" s="32">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="U9" s="32">
         <v>45</v>
@@ -31892,7 +31921,7 @@
         <v>45</v>
       </c>
       <c r="W9" s="32">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="X9" s="32">
         <v>24</v>
@@ -31906,117 +31935,124 @@
       <c r="AA9" s="32">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB9" s="32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="31">
-        <f t="shared" ref="B10:Z10" si="6">(B8+B9)/2</f>
+        <f t="shared" ref="B10:AA10" si="8">(B8+B9)/2</f>
         <v>55</v>
       </c>
       <c r="C10" s="32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
       <c r="D10" s="32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
       <c r="E10" s="32">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E10" si="9">(E8+E9)/2</f>
+        <v>40</v>
+      </c>
+      <c r="F10" s="32">
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
-      <c r="F10" s="32">
-        <f t="shared" si="6"/>
+      <c r="G10" s="32">
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="G10" s="32">
-        <f t="shared" si="6"/>
+      <c r="H10" s="32">
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="H10" s="32">
-        <f t="shared" si="6"/>
+      <c r="I10" s="32">
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="I10" s="32">
-        <f t="shared" si="6"/>
+      <c r="J10" s="32">
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="J10" s="32">
-        <f t="shared" ref="J10" si="7">(J8+J9)/2</f>
+      <c r="K10" s="32">
+        <f t="shared" ref="K10" si="10">(K8+K9)/2</f>
         <v>37</v>
       </c>
-      <c r="K10" s="32">
-        <f t="shared" si="6"/>
+      <c r="L10" s="32">
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="L10" s="32">
-        <f t="shared" si="6"/>
+      <c r="M10" s="32">
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="M10" s="32">
-        <f t="shared" si="6"/>
+      <c r="N10" s="32">
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="N10" s="32">
-        <f t="shared" si="6"/>
+      <c r="O10" s="32">
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="O10" s="32">
-        <f t="shared" si="6"/>
+      <c r="P10" s="32">
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="P10" s="32">
-        <f t="shared" si="6"/>
+      <c r="Q10" s="32">
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
-      <c r="Q10" s="32">
-        <f t="shared" si="6"/>
+      <c r="R10" s="32">
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="R10" s="32">
-        <f t="shared" si="6"/>
+      <c r="S10" s="32">
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="S10" s="32">
-        <f t="shared" si="6"/>
+      <c r="T10" s="32">
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="T10" s="32">
-        <f t="shared" si="6"/>
+      <c r="U10" s="32">
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="U10" s="32">
-        <f t="shared" si="6"/>
+      <c r="V10" s="32">
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="V10" s="32">
-        <f t="shared" si="6"/>
+      <c r="W10" s="32">
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="W10" s="32">
-        <f t="shared" si="6"/>
+      <c r="X10" s="32">
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="X10" s="32">
-        <f t="shared" si="6"/>
+      <c r="Y10" s="32">
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="Y10" s="32">
-        <f t="shared" si="6"/>
+      <c r="Z10" s="32">
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="Z10" s="32">
-        <f t="shared" si="6"/>
+      <c r="AA10" s="32">
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="AA10" s="32">
-        <f t="shared" ref="AA10" si="8">(AA8+AA9)/2</f>
+      <c r="AB10" s="32">
+        <f t="shared" ref="AB10" si="11">(AB8+AB9)/2</f>
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>42</v>
       </c>
@@ -32039,7 +32075,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="32">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I11" s="32">
         <v>45</v>
@@ -32048,7 +32084,7 @@
         <v>45</v>
       </c>
       <c r="K11" s="32">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="L11" s="32">
         <v>25</v>
@@ -32063,10 +32099,10 @@
         <v>25</v>
       </c>
       <c r="P11" s="32">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="32">
         <v>35</v>
-      </c>
-      <c r="Q11" s="32">
-        <v>30</v>
       </c>
       <c r="R11" s="32">
         <v>30</v>
@@ -32075,7 +32111,7 @@
         <v>30</v>
       </c>
       <c r="T11" s="32">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="U11" s="32">
         <v>20</v>
@@ -32084,7 +32120,7 @@
         <v>20</v>
       </c>
       <c r="W11" s="32">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="X11" s="32">
         <v>30</v>
@@ -32098,8 +32134,11 @@
       <c r="AA11" s="32">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB11" s="32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>43</v>
       </c>
@@ -32122,7 +32161,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="32">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="I12" s="32">
         <v>35</v>
@@ -32131,7 +32170,7 @@
         <v>35</v>
       </c>
       <c r="K12" s="32">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="L12" s="32">
         <v>15</v>
@@ -32146,10 +32185,10 @@
         <v>15</v>
       </c>
       <c r="P12" s="32">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="32">
         <v>25</v>
-      </c>
-      <c r="Q12" s="32">
-        <v>20</v>
       </c>
       <c r="R12" s="32">
         <v>20</v>
@@ -32158,7 +32197,7 @@
         <v>20</v>
       </c>
       <c r="T12" s="32">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="U12" s="32">
         <v>10</v>
@@ -32167,7 +32206,7 @@
         <v>10</v>
       </c>
       <c r="W12" s="32">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="X12" s="32">
         <v>20</v>
@@ -32181,117 +32220,124 @@
       <c r="AA12" s="32">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB12" s="32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="31">
-        <f t="shared" ref="B13:Z13" si="9">(B11+B12)/2</f>
+        <f t="shared" ref="B13:AA13" si="12">(B11+B12)/2</f>
         <v>15</v>
       </c>
       <c r="C13" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="D13" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="E13" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="E13" si="13">(E11+E12)/2</f>
         <v>10</v>
       </c>
       <c r="F13" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="G13" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="H13" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="I13" s="32">
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
-      <c r="I13" s="32">
-        <f t="shared" si="9"/>
+      <c r="J13" s="32">
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
-      <c r="J13" s="32">
-        <f t="shared" ref="J13" si="10">(J11+J12)/2</f>
+      <c r="K13" s="32">
+        <f t="shared" ref="K13" si="14">(K11+K12)/2</f>
         <v>40</v>
       </c>
-      <c r="K13" s="32">
-        <f t="shared" si="9"/>
+      <c r="L13" s="32">
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
-      <c r="L13" s="32">
-        <f t="shared" si="9"/>
+      <c r="M13" s="32">
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
-      <c r="M13" s="32">
-        <f t="shared" si="9"/>
+      <c r="N13" s="32">
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
-      <c r="N13" s="32">
-        <f t="shared" si="9"/>
+      <c r="O13" s="32">
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
-      <c r="O13" s="32">
-        <f t="shared" si="9"/>
+      <c r="P13" s="32">
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
-      <c r="P13" s="32">
-        <f t="shared" si="9"/>
+      <c r="Q13" s="32">
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
-      <c r="Q13" s="32">
-        <f t="shared" si="9"/>
+      <c r="R13" s="32">
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="R13" s="32">
-        <f t="shared" si="9"/>
+      <c r="S13" s="32">
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="S13" s="32">
-        <f t="shared" si="9"/>
+      <c r="T13" s="32">
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="T13" s="32">
-        <f t="shared" si="9"/>
+      <c r="U13" s="32">
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="U13" s="32">
-        <f t="shared" si="9"/>
+      <c r="V13" s="32">
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="V13" s="32">
-        <f t="shared" si="9"/>
+      <c r="W13" s="32">
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="W13" s="32">
-        <f t="shared" si="9"/>
+      <c r="X13" s="32">
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="X13" s="32">
-        <f t="shared" si="9"/>
+      <c r="Y13" s="32">
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="Y13" s="32">
-        <f t="shared" si="9"/>
+      <c r="Z13" s="32">
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="Z13" s="32">
-        <f t="shared" si="9"/>
+      <c r="AA13" s="32">
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="AA13" s="32">
-        <f t="shared" ref="AA13" si="11">(AA11+AA12)/2</f>
+      <c r="AB13" s="32">
+        <f t="shared" ref="AB13" si="15">(AB11+AB12)/2</f>
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
         <v>44</v>
       </c>
@@ -32373,8 +32419,11 @@
       <c r="AA14" s="32">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB14" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>45</v>
       </c>
@@ -32456,117 +32505,124 @@
       <c r="AA15" s="32">
         <v>-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB15" s="32">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="31">
-        <f t="shared" ref="B16:Z16" si="12">(B14+B15)/2</f>
+        <f t="shared" ref="B16:AA16" si="16">(B14+B15)/2</f>
         <v>0</v>
       </c>
       <c r="C16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="D16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="E16" si="17">(E14+E15)/2</f>
         <v>0</v>
       </c>
       <c r="F16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J16" s="32">
-        <f t="shared" ref="J16" si="13">(J14+J15)/2</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="K16" si="18">(K14+K15)/2</f>
         <v>0</v>
       </c>
       <c r="L16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="S16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="T16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="V16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Y16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Z16" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA16" s="32">
-        <f t="shared" ref="AA16" si="14">(AA14+AA15)/2</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB16" s="32">
+        <f t="shared" ref="AB16" si="19">(AB14+AB15)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>16</v>
       </c>
@@ -32580,7 +32636,7 @@
         <v>29</v>
       </c>
       <c r="E17" s="32">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F17" s="32">
         <v>31</v>
@@ -32589,7 +32645,7 @@
         <v>31</v>
       </c>
       <c r="H17" s="32">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="I17" s="32">
         <v>24</v>
@@ -32598,7 +32654,7 @@
         <v>24</v>
       </c>
       <c r="K17" s="32">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="L17" s="32">
         <v>37</v>
@@ -32613,7 +32669,7 @@
         <v>37</v>
       </c>
       <c r="P17" s="32">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Q17" s="32">
         <v>34</v>
@@ -32625,7 +32681,7 @@
         <v>34</v>
       </c>
       <c r="T17" s="32">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="U17" s="32">
         <v>31</v>
@@ -32634,7 +32690,7 @@
         <v>31</v>
       </c>
       <c r="W17" s="32">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="X17" s="32">
         <v>34</v>
@@ -32648,8 +32704,11 @@
       <c r="AA17" s="32">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB17" s="32">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
       <c r="B18" s="43"/>
       <c r="C18" s="43"/>
@@ -32677,113 +32736,118 @@
       <c r="Y18" s="43"/>
       <c r="Z18" s="43"/>
       <c r="AA18" s="43"/>
-    </row>
-    <row r="19" spans="1:27" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB18" s="43"/>
+    </row>
+    <row r="19" spans="1:28" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="32">
-        <f t="shared" ref="B19:Z19" si="15">B4+B7+B10+B13+B16+B17</f>
+        <f t="shared" ref="B19:AA19" si="20">B4+B7+B10+B13+B16+B17</f>
         <v>265</v>
       </c>
       <c r="C19" s="32">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>204</v>
       </c>
       <c r="D19" s="32">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>199</v>
       </c>
       <c r="E19" s="32">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="E19" si="21">E4+E7+E10+E13+E16+E17</f>
+        <v>204</v>
+      </c>
+      <c r="F19" s="32">
+        <f t="shared" si="20"/>
         <v>266</v>
       </c>
-      <c r="F19" s="32">
-        <f t="shared" si="15"/>
+      <c r="G19" s="32">
+        <f t="shared" si="20"/>
         <v>266</v>
       </c>
-      <c r="G19" s="32">
-        <f t="shared" si="15"/>
+      <c r="H19" s="32">
+        <f t="shared" si="20"/>
         <v>266</v>
       </c>
-      <c r="H19" s="32">
-        <f t="shared" si="15"/>
+      <c r="I19" s="32">
+        <f t="shared" si="20"/>
         <v>261</v>
       </c>
-      <c r="I19" s="32">
-        <f t="shared" ref="I19:J19" si="16">I4+I7+I10+I13+I16+I17</f>
+      <c r="J19" s="32">
+        <f t="shared" ref="J19:K19" si="22">J4+J7+J10+J13+J16+J17</f>
         <v>261</v>
       </c>
-      <c r="J19" s="32">
-        <f t="shared" si="16"/>
+      <c r="K19" s="32">
+        <f t="shared" si="22"/>
         <v>261</v>
       </c>
-      <c r="K19" s="32">
-        <f t="shared" si="15"/>
+      <c r="L19" s="32">
+        <f t="shared" si="20"/>
         <v>244</v>
       </c>
-      <c r="L19" s="32">
-        <f t="shared" si="15"/>
+      <c r="M19" s="32">
+        <f t="shared" si="20"/>
         <v>244</v>
       </c>
-      <c r="M19" s="32">
-        <f t="shared" si="15"/>
+      <c r="N19" s="32">
+        <f t="shared" si="20"/>
         <v>244</v>
       </c>
-      <c r="N19" s="32">
-        <f t="shared" si="15"/>
+      <c r="O19" s="32">
+        <f t="shared" si="20"/>
         <v>244</v>
       </c>
-      <c r="O19" s="32">
-        <f t="shared" si="15"/>
+      <c r="P19" s="32">
+        <f t="shared" si="20"/>
         <v>244</v>
       </c>
-      <c r="P19" s="32">
-        <f t="shared" si="15"/>
+      <c r="Q19" s="32">
+        <f t="shared" si="20"/>
         <v>246</v>
       </c>
-      <c r="Q19" s="32">
-        <f t="shared" si="15"/>
+      <c r="R19" s="32">
+        <f t="shared" si="20"/>
         <v>251</v>
       </c>
-      <c r="R19" s="32">
-        <f t="shared" si="15"/>
+      <c r="S19" s="32">
+        <f t="shared" si="20"/>
         <v>251</v>
       </c>
-      <c r="S19" s="32">
-        <f t="shared" si="15"/>
+      <c r="T19" s="32">
+        <f t="shared" si="20"/>
         <v>251</v>
       </c>
-      <c r="T19" s="32">
-        <f t="shared" si="15"/>
+      <c r="U19" s="32">
+        <f t="shared" si="20"/>
         <v>266</v>
       </c>
-      <c r="U19" s="32">
-        <f t="shared" si="15"/>
+      <c r="V19" s="32">
+        <f t="shared" si="20"/>
         <v>266</v>
       </c>
-      <c r="V19" s="32">
-        <f t="shared" si="15"/>
+      <c r="W19" s="32">
+        <f t="shared" si="20"/>
         <v>266</v>
       </c>
-      <c r="W19" s="32">
-        <f t="shared" si="15"/>
+      <c r="X19" s="32">
+        <f t="shared" si="20"/>
         <v>236</v>
       </c>
-      <c r="X19" s="32">
-        <f t="shared" si="15"/>
+      <c r="Y19" s="32">
+        <f t="shared" si="20"/>
         <v>236</v>
       </c>
-      <c r="Y19" s="32">
-        <f t="shared" si="15"/>
+      <c r="Z19" s="32">
+        <f t="shared" si="20"/>
         <v>236</v>
       </c>
-      <c r="Z19" s="32">
-        <f t="shared" si="15"/>
+      <c r="AA19" s="32">
+        <f t="shared" si="20"/>
         <v>236</v>
       </c>
-      <c r="AA19" s="32">
-        <f t="shared" ref="AA19" si="17">AA4+AA7+AA10+AA13+AA16+AA17</f>
+      <c r="AB19" s="32">
+        <f t="shared" ref="AB19" si="23">AB4+AB7+AB10+AB13+AB16+AB17</f>
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Water Elemental and Mage Water and Necromancer
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67E74E0-1101-4227-AC41-2CAFF7CDED0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC561169-0C5F-4BE1-B177-2EB07873E472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14625" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31089,7 +31089,7 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31211,7 +31211,7 @@
         <v>60</v>
       </c>
       <c r="E2" s="22">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F2" s="22">
         <v>115</v>
@@ -31297,7 +31297,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="22">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F3" s="22">
         <v>105</v>
@@ -31387,7 +31387,7 @@
       </c>
       <c r="E4" s="22">
         <f t="shared" ref="E4" si="1">(E2+E3)/2</f>
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F4" s="22">
         <f t="shared" si="0"/>
@@ -31496,7 +31496,7 @@
         <v>70</v>
       </c>
       <c r="E5" s="22">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F5" s="22">
         <v>75</v>
@@ -31582,7 +31582,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="40">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F6" s="40">
         <v>65</v>
@@ -31672,7 +31672,7 @@
       </c>
       <c r="E7" s="32">
         <f t="shared" ref="E7" si="5">(E5+E6)/2</f>
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F7" s="32">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Warrior Weapon Master update
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6164A42-523D-4165-87E6-F1B89C0D5A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56513D3-C93F-4B76-BFE0-C4B4728F513A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14175" yWindow="-16440" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bar" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Warrior_Comprehensiveness</t>
-  </si>
-  <si>
-    <t>Warrior_Skeleton</t>
   </si>
   <si>
     <t>Warrior_Void_Rambler</t>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>Warrior_Defence</t>
+  </si>
+  <si>
+    <t>Warrior_Weapon_Master</t>
   </si>
 </sst>
 </file>
@@ -710,10 +710,10 @@
                   <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.81818181818181823</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.375</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.67567567567567566</c:v>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B4" s="16">
         <f t="shared" ref="B4:M4" si="2">B10/$N10</f>
-        <v>1</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="2"/>
@@ -3143,7 +3143,7 @@
       </c>
       <c r="B5" s="16">
         <f t="shared" ref="B5:M5" si="3">B11/$N11</f>
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="3"/>
@@ -3439,7 +3439,7 @@
       </c>
       <c r="B10" s="22">
         <f>'Property List'!B10</f>
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C10" s="22">
         <f>'Property List'!G10</f>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="B11" s="22">
         <f>'Property List'!B13</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C11" s="22">
         <f>'Property List'!G13</f>
@@ -31092,14 +31092,13 @@
   <dimension ref="A1:AC19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="27.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="27.88671875" style="1" customWidth="1"/>
     <col min="5" max="6" width="26.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="32" style="1" customWidth="1"/>
     <col min="8" max="10" width="26" style="1" customWidth="1"/>
@@ -31122,70 +31121,70 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="Y1" s="29" t="s">
         <v>8</v>
@@ -31200,21 +31199,21 @@
         <v>11</v>
       </c>
       <c r="AC1" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="22">
         <v>105</v>
       </c>
       <c r="C2" s="22">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D2" s="22">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="E2" s="22">
         <v>60</v>
@@ -31294,16 +31293,16 @@
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="22">
         <v>95</v>
       </c>
       <c r="C3" s="22">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D3" s="22">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E3" s="22">
         <v>50</v>
@@ -31390,19 +31389,19 @@
         <v>100</v>
       </c>
       <c r="C4" s="22">
-        <f t="shared" ref="C4" si="1">(C2+C3)/2</f>
-        <v>100</v>
+        <f t="shared" ref="C4:D4" si="1">(C2+C3)/2</f>
+        <v>105</v>
       </c>
       <c r="D4" s="22">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <f t="shared" ref="D4" si="2">(D2+D3)/2</f>
+        <v>95</v>
       </c>
       <c r="E4" s="22">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="F4" s="22">
-        <f t="shared" ref="F4" si="2">(F2+F3)/2</f>
+        <f t="shared" ref="F4" si="3">(F2+F3)/2</f>
         <v>70</v>
       </c>
       <c r="G4" s="22">
@@ -31426,7 +31425,7 @@
         <v>80</v>
       </c>
       <c r="L4" s="22">
-        <f t="shared" ref="L4" si="3">(L2+L3)/2</f>
+        <f t="shared" ref="L4" si="4">(L2+L3)/2</f>
         <v>80</v>
       </c>
       <c r="M4" s="22">
@@ -31494,22 +31493,22 @@
         <v>75</v>
       </c>
       <c r="AC4" s="34">
-        <f t="shared" ref="AC4" si="4">(AC2+AC3)/2</f>
+        <f t="shared" ref="AC4" si="5">(AC2+AC3)/2</f>
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="22">
         <v>75</v>
       </c>
       <c r="C5" s="22">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D5" s="22">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E5" s="22">
         <v>70</v>
@@ -31589,16 +31588,16 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="39">
         <v>65</v>
       </c>
       <c r="C6" s="39">
-        <v>65</v>
-      </c>
-      <c r="D6" s="40">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="D6" s="39">
+        <v>70</v>
       </c>
       <c r="E6" s="40">
         <v>60</v>
@@ -31681,130 +31680,130 @@
         <v>13</v>
       </c>
       <c r="B7" s="31">
-        <f t="shared" ref="B7:AB7" si="5">(B5+B6)/2</f>
+        <f t="shared" ref="B7:AB7" si="6">(B5+B6)/2</f>
         <v>70</v>
       </c>
       <c r="C7" s="31">
-        <f t="shared" ref="C7" si="6">(C5+C6)/2</f>
+        <f t="shared" ref="C7:D7" si="7">(C5+C6)/2</f>
+        <v>65</v>
+      </c>
+      <c r="D7" s="31">
+        <f t="shared" ref="D7" si="8">(D5+D6)/2</f>
+        <v>75</v>
+      </c>
+      <c r="E7" s="32">
+        <f t="shared" si="6"/>
+        <v>65</v>
+      </c>
+      <c r="F7" s="32">
+        <f t="shared" ref="F7" si="9">(F5+F6)/2</f>
+        <v>55</v>
+      </c>
+      <c r="G7" s="32">
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
-      <c r="D7" s="32">
-        <f t="shared" si="5"/>
+      <c r="H7" s="32">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="6"/>
+        <v>65</v>
+      </c>
+      <c r="J7" s="32">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="K7" s="32">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="L7" s="32">
+        <f t="shared" ref="L7" si="10">(L5+L6)/2</f>
+        <v>80</v>
+      </c>
+      <c r="M7" s="32">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="N7" s="32">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="O7" s="32">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="P7" s="32">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="Q7" s="32">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="R7" s="32">
+        <f t="shared" si="6"/>
+        <v>65</v>
+      </c>
+      <c r="S7" s="32">
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
-      <c r="E7" s="32">
-        <f t="shared" si="5"/>
+      <c r="T7" s="32">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="U7" s="32">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="V7" s="32">
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
-      <c r="F7" s="32">
-        <f t="shared" ref="F7" si="7">(F5+F6)/2</f>
-        <v>55</v>
-      </c>
-      <c r="G7" s="32">
-        <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="H7" s="32">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="I7" s="32">
-        <f t="shared" si="5"/>
+      <c r="W7" s="32">
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
-      <c r="J7" s="32">
-        <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="K7" s="32">
-        <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="L7" s="32">
-        <f t="shared" ref="L7" si="8">(L5+L6)/2</f>
-        <v>80</v>
-      </c>
-      <c r="M7" s="32">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="N7" s="32">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="O7" s="32">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="P7" s="32">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="Q7" s="32">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="R7" s="32">
-        <f t="shared" si="5"/>
+      <c r="X7" s="32">
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
-      <c r="S7" s="32">
-        <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="T7" s="32">
-        <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="U7" s="32">
-        <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="V7" s="32">
-        <f t="shared" si="5"/>
-        <v>65</v>
-      </c>
-      <c r="W7" s="32">
-        <f t="shared" si="5"/>
-        <v>65</v>
-      </c>
-      <c r="X7" s="32">
-        <f t="shared" si="5"/>
-        <v>65</v>
-      </c>
       <c r="Y7" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="Z7" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="AA7" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="AB7" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="AC7" s="32">
-        <f t="shared" ref="AC7" si="9">(AC5+AC6)/2</f>
+        <f t="shared" ref="AC7" si="11">(AC5+AC6)/2</f>
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="31">
+        <v>50</v>
+      </c>
+      <c r="C8" s="31">
+        <v>65</v>
+      </c>
+      <c r="D8" s="31">
         <v>60</v>
-      </c>
-      <c r="C8" s="31">
-        <v>60</v>
-      </c>
-      <c r="D8" s="32">
-        <v>50</v>
       </c>
       <c r="E8" s="32">
         <v>50</v>
@@ -31884,16 +31883,16 @@
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="31">
+        <v>40</v>
+      </c>
+      <c r="C9" s="31">
+        <v>55</v>
+      </c>
+      <c r="D9" s="31">
         <v>50</v>
-      </c>
-      <c r="C9" s="31">
-        <v>50</v>
-      </c>
-      <c r="D9" s="32">
-        <v>40</v>
       </c>
       <c r="E9" s="32">
         <v>40</v>
@@ -31976,130 +31975,130 @@
         <v>14</v>
       </c>
       <c r="B10" s="31">
-        <f t="shared" ref="B10:AB10" si="10">(B8+B9)/2</f>
+        <f t="shared" ref="B10:AB10" si="12">(B8+B9)/2</f>
+        <v>45</v>
+      </c>
+      <c r="C10" s="31">
+        <f t="shared" ref="C10:D10" si="13">(C8+C9)/2</f>
+        <v>60</v>
+      </c>
+      <c r="D10" s="31">
+        <f t="shared" ref="D10" si="14">(D8+D9)/2</f>
         <v>55</v>
       </c>
-      <c r="C10" s="31">
-        <f t="shared" ref="C10" si="11">(C8+C9)/2</f>
-        <v>55</v>
-      </c>
-      <c r="D10" s="32">
-        <f t="shared" si="10"/>
+      <c r="E10" s="32">
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
-      <c r="E10" s="32">
-        <f t="shared" si="10"/>
+      <c r="F10" s="32">
+        <f t="shared" ref="F10" si="15">(F8+F9)/2</f>
+        <v>40</v>
+      </c>
+      <c r="G10" s="32">
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
-      <c r="F10" s="32">
-        <f t="shared" ref="F10" si="12">(F8+F9)/2</f>
-        <v>40</v>
-      </c>
-      <c r="G10" s="32">
-        <f t="shared" si="10"/>
-        <v>45</v>
-      </c>
       <c r="H10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="I10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="J10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="K10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="L10" s="32">
-        <f t="shared" ref="L10" si="13">(L8+L9)/2</f>
+        <f t="shared" ref="L10" si="16">(L8+L9)/2</f>
         <v>37</v>
       </c>
       <c r="M10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="N10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="O10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="P10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="Q10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="R10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>32</v>
       </c>
       <c r="S10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>27</v>
       </c>
       <c r="T10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>27</v>
       </c>
       <c r="U10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>27</v>
       </c>
       <c r="V10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="W10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="X10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="Y10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>27</v>
       </c>
       <c r="Z10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>27</v>
       </c>
       <c r="AA10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>27</v>
       </c>
       <c r="AB10" s="32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>27</v>
       </c>
       <c r="AC10" s="32">
-        <f t="shared" ref="AC10" si="14">(AC8+AC9)/2</f>
+        <f t="shared" ref="AC10" si="17">(AC8+AC9)/2</f>
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="31">
+        <v>30</v>
+      </c>
+      <c r="C11" s="31">
+        <v>15</v>
+      </c>
+      <c r="D11" s="31">
         <v>20</v>
-      </c>
-      <c r="C11" s="31">
-        <v>20</v>
-      </c>
-      <c r="D11" s="32">
-        <v>15</v>
       </c>
       <c r="E11" s="32">
         <v>10</v>
@@ -32179,16 +32178,16 @@
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="31">
+        <v>20</v>
+      </c>
+      <c r="C12" s="31">
+        <v>5</v>
+      </c>
+      <c r="D12" s="31">
         <v>10</v>
-      </c>
-      <c r="C12" s="31">
-        <v>10</v>
-      </c>
-      <c r="D12" s="32">
-        <v>5</v>
       </c>
       <c r="E12" s="32">
         <v>0</v>
@@ -32271,121 +32270,121 @@
         <v>15</v>
       </c>
       <c r="B13" s="31">
-        <f t="shared" ref="B13:AB13" si="15">(B11+B12)/2</f>
+        <f t="shared" ref="B13:AB13" si="18">(B11+B12)/2</f>
+        <v>25</v>
+      </c>
+      <c r="C13" s="31">
+        <f t="shared" ref="C13:D13" si="19">(C11+C12)/2</f>
+        <v>10</v>
+      </c>
+      <c r="D13" s="31">
+        <f t="shared" ref="D13" si="20">(D11+D12)/2</f>
         <v>15</v>
       </c>
-      <c r="C13" s="31">
-        <f t="shared" ref="C13" si="16">(C11+C12)/2</f>
+      <c r="E13" s="32">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="F13" s="32">
+        <f t="shared" ref="F13" si="21">(F11+F12)/2</f>
+        <v>10</v>
+      </c>
+      <c r="G13" s="32">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="H13" s="32">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="I13" s="32">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="J13" s="32">
+        <f t="shared" si="18"/>
+        <v>40</v>
+      </c>
+      <c r="K13" s="32">
+        <f t="shared" si="18"/>
+        <v>40</v>
+      </c>
+      <c r="L13" s="32">
+        <f t="shared" ref="L13" si="22">(L11+L12)/2</f>
+        <v>40</v>
+      </c>
+      <c r="M13" s="32">
+        <f t="shared" si="18"/>
+        <v>20</v>
+      </c>
+      <c r="N13" s="32">
+        <f t="shared" si="18"/>
+        <v>20</v>
+      </c>
+      <c r="O13" s="32">
+        <f t="shared" si="18"/>
+        <v>20</v>
+      </c>
+      <c r="P13" s="32">
+        <f t="shared" si="18"/>
+        <v>20</v>
+      </c>
+      <c r="Q13" s="32">
+        <f t="shared" si="18"/>
+        <v>20</v>
+      </c>
+      <c r="R13" s="32">
+        <f t="shared" si="18"/>
+        <v>30</v>
+      </c>
+      <c r="S13" s="32">
+        <f t="shared" si="18"/>
+        <v>25</v>
+      </c>
+      <c r="T13" s="32">
+        <f t="shared" si="18"/>
+        <v>25</v>
+      </c>
+      <c r="U13" s="32">
+        <f t="shared" si="18"/>
+        <v>25</v>
+      </c>
+      <c r="V13" s="32">
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
-      <c r="D13" s="32">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E13" s="32">
-        <f t="shared" si="15"/>
-        <v>5</v>
-      </c>
-      <c r="F13" s="32">
-        <f t="shared" ref="F13" si="17">(F11+F12)/2</f>
-        <v>10</v>
-      </c>
-      <c r="G13" s="32">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="H13" s="32">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="I13" s="32">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="J13" s="32">
-        <f t="shared" si="15"/>
-        <v>40</v>
-      </c>
-      <c r="K13" s="32">
-        <f t="shared" si="15"/>
-        <v>40</v>
-      </c>
-      <c r="L13" s="32">
-        <f t="shared" ref="L13" si="18">(L11+L12)/2</f>
-        <v>40</v>
-      </c>
-      <c r="M13" s="32">
-        <f t="shared" si="15"/>
-        <v>20</v>
-      </c>
-      <c r="N13" s="32">
-        <f t="shared" si="15"/>
-        <v>20</v>
-      </c>
-      <c r="O13" s="32">
-        <f t="shared" si="15"/>
-        <v>20</v>
-      </c>
-      <c r="P13" s="32">
-        <f t="shared" si="15"/>
-        <v>20</v>
-      </c>
-      <c r="Q13" s="32">
-        <f t="shared" si="15"/>
-        <v>20</v>
-      </c>
-      <c r="R13" s="32">
-        <f t="shared" si="15"/>
-        <v>30</v>
-      </c>
-      <c r="S13" s="32">
-        <f t="shared" si="15"/>
+      <c r="W13" s="32">
+        <f t="shared" si="18"/>
+        <v>15</v>
+      </c>
+      <c r="X13" s="32">
+        <f t="shared" si="18"/>
+        <v>15</v>
+      </c>
+      <c r="Y13" s="32">
+        <f t="shared" si="18"/>
         <v>25</v>
       </c>
-      <c r="T13" s="32">
-        <f t="shared" si="15"/>
+      <c r="Z13" s="32">
+        <f t="shared" si="18"/>
         <v>25</v>
       </c>
-      <c r="U13" s="32">
-        <f t="shared" si="15"/>
+      <c r="AA13" s="32">
+        <f t="shared" si="18"/>
         <v>25</v>
       </c>
-      <c r="V13" s="32">
-        <f t="shared" si="15"/>
-        <v>15</v>
-      </c>
-      <c r="W13" s="32">
-        <f t="shared" si="15"/>
-        <v>15</v>
-      </c>
-      <c r="X13" s="32">
-        <f t="shared" si="15"/>
-        <v>15</v>
-      </c>
-      <c r="Y13" s="32">
-        <f t="shared" si="15"/>
+      <c r="AB13" s="32">
+        <f t="shared" si="18"/>
         <v>25</v>
       </c>
-      <c r="Z13" s="32">
-        <f t="shared" si="15"/>
-        <v>25</v>
-      </c>
-      <c r="AA13" s="32">
-        <f t="shared" si="15"/>
-        <v>25</v>
-      </c>
-      <c r="AB13" s="32">
-        <f t="shared" si="15"/>
-        <v>25</v>
-      </c>
       <c r="AC13" s="32">
-        <f t="shared" ref="AC13" si="19">(AC11+AC12)/2</f>
+        <f t="shared" ref="AC13" si="23">(AC11+AC12)/2</f>
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="31">
         <v>5</v>
@@ -32393,7 +32392,7 @@
       <c r="C14" s="31">
         <v>5</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="31">
         <v>5</v>
       </c>
       <c r="E14" s="32">
@@ -32474,7 +32473,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="31">
         <v>-5</v>
@@ -32482,7 +32481,7 @@
       <c r="C15" s="31">
         <v>-5</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="31">
         <v>-5</v>
       </c>
       <c r="E15" s="32">
@@ -32563,118 +32562,118 @@
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="31">
-        <f t="shared" ref="B16:AB16" si="20">(B14+B15)/2</f>
+        <f t="shared" ref="B16:AB16" si="24">(B14+B15)/2</f>
         <v>0</v>
       </c>
       <c r="C16" s="31">
-        <f t="shared" ref="C16" si="21">(C14+C15)/2</f>
+        <f t="shared" ref="C16:D16" si="25">(C14+C15)/2</f>
         <v>0</v>
       </c>
-      <c r="D16" s="32">
-        <f t="shared" si="20"/>
+      <c r="D16" s="31">
+        <f t="shared" ref="D16" si="26">(D14+D15)/2</f>
         <v>0</v>
       </c>
       <c r="E16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="F16" s="32">
-        <f t="shared" ref="F16" si="22">(F14+F15)/2</f>
+        <f t="shared" ref="F16" si="27">(F14+F15)/2</f>
         <v>0</v>
       </c>
       <c r="G16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L16" s="32">
-        <f t="shared" ref="L16" si="23">(L14+L15)/2</f>
+        <f t="shared" ref="L16" si="28">(L14+L15)/2</f>
         <v>0</v>
       </c>
       <c r="M16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="P16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="R16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="S16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="T16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="U16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="W16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="X16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Y16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Z16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AA16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AB16" s="32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AC16" s="32">
-        <f t="shared" ref="AC16" si="24">(AC14+AC15)/2</f>
+        <f t="shared" ref="AC16" si="29">(AC14+AC15)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -32688,8 +32687,8 @@
       <c r="C17" s="31">
         <v>25</v>
       </c>
-      <c r="D17" s="32">
-        <v>29</v>
+      <c r="D17" s="31">
+        <v>25</v>
       </c>
       <c r="E17" s="32">
         <v>29</v>
@@ -32800,118 +32799,118 @@
     </row>
     <row r="19" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="32">
-        <f t="shared" ref="B19:AB19" si="25">B4+B7+B10+B13+B16+B17</f>
+        <f t="shared" ref="B19:AB19" si="30">B4+B7+B10+B13+B16+B17</f>
         <v>265</v>
       </c>
       <c r="C19" s="32">
-        <f t="shared" ref="C19" si="26">C4+C7+C10+C13+C16+C17</f>
+        <f t="shared" ref="C19:D19" si="31">C4+C7+C10+C13+C16+C17</f>
         <v>265</v>
       </c>
       <c r="D19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="D19" si="32">D4+D7+D10+D13+D16+D17</f>
+        <v>265</v>
+      </c>
+      <c r="E19" s="32">
+        <f t="shared" si="30"/>
+        <v>199</v>
+      </c>
+      <c r="F19" s="32">
+        <f t="shared" ref="F19" si="33">F4+F7+F10+F13+F16+F17</f>
         <v>204</v>
       </c>
-      <c r="E19" s="32">
-        <f t="shared" si="25"/>
-        <v>199</v>
-      </c>
-      <c r="F19" s="32">
-        <f t="shared" ref="F19" si="27">F4+F7+F10+F13+F16+F17</f>
-        <v>204</v>
-      </c>
       <c r="G19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>266</v>
       </c>
       <c r="H19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>266</v>
       </c>
       <c r="I19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>266</v>
       </c>
       <c r="J19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>261</v>
       </c>
       <c r="K19" s="32">
-        <f t="shared" ref="K19:L19" si="28">K4+K7+K10+K13+K16+K17</f>
+        <f t="shared" ref="K19:L19" si="34">K4+K7+K10+K13+K16+K17</f>
         <v>261</v>
       </c>
       <c r="L19" s="32">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>261</v>
       </c>
       <c r="M19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>244</v>
       </c>
       <c r="N19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>244</v>
       </c>
       <c r="O19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>244</v>
       </c>
       <c r="P19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>244</v>
       </c>
       <c r="Q19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>244</v>
       </c>
       <c r="R19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>246</v>
       </c>
       <c r="S19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>251</v>
       </c>
       <c r="T19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>251</v>
       </c>
       <c r="U19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>251</v>
       </c>
       <c r="V19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>266</v>
       </c>
       <c r="W19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>266</v>
       </c>
       <c r="X19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>266</v>
       </c>
       <c r="Y19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>236</v>
       </c>
       <c r="Z19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>236</v>
       </c>
       <c r="AA19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>236</v>
       </c>
       <c r="AB19" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>236</v>
       </c>
       <c r="AC19" s="32">
-        <f t="shared" ref="AC19" si="29">AC4+AC7+AC10+AC13+AC16+AC17</f>
+        <f t="shared" ref="AC19" si="35">AC4+AC7+AC10+AC13+AC16+AC17</f>
         <v>236</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Warrior Weapon Master updated
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E27C795-EC0D-4E4C-87A8-3A2546388C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0843D502-159B-4F3D-A1B4-D2D7C1DABD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17295" yWindow="-14445" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14625" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bar" sheetId="1" r:id="rId1"/>
@@ -1427,10 +1427,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.68181818181818177</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9375</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.49090909090909091</c:v>
@@ -1587,16 +1587,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.68181818181818177</c:v>
+                  <c:v>0.72727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9375</c:v>
+                  <c:v>0.8125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.49090909090909091</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.625</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.91891891891891897</c:v>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="K2" s="12">
         <f t="shared" si="0"/>
-        <v>0.68181818181818177</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="L2" s="12">
         <f t="shared" si="0"/>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="M2" s="13">
         <f t="shared" si="0"/>
-        <v>0.68181818181818177</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="K3" s="12">
         <f t="shared" si="1"/>
-        <v>0.9375</v>
+        <v>1</v>
       </c>
       <c r="L3" s="12">
         <f t="shared" si="1"/>
@@ -3058,7 +3058,7 @@
       </c>
       <c r="M3" s="13">
         <f t="shared" si="1"/>
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
@@ -3190,7 +3190,7 @@
       </c>
       <c r="M5" s="13">
         <f t="shared" si="3"/>
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="K8" s="23">
         <f>'Property List'!AA4</f>
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="L8" s="23">
         <f>'Property List'!AB4</f>
@@ -3350,7 +3350,7 @@
       </c>
       <c r="M8" s="23">
         <f>'Property List'!AC4</f>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="N8" s="24">
         <v>110</v>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="K9" s="23">
         <f>'Property List'!AA7</f>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L9" s="23">
         <f>'Property List'!AB7</f>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="M9" s="23">
         <f>'Property List'!AC7</f>
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="N9" s="24">
         <v>80</v>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="M11" s="23">
         <f>'Property List'!AC13</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="N11" s="24">
         <v>40</v>
@@ -31095,7 +31095,10 @@
   <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31288,13 +31291,13 @@
         <v>80</v>
       </c>
       <c r="AA2" s="22">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AB2" s="22">
         <v>80</v>
       </c>
       <c r="AC2" s="34">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AD2" s="34">
         <v>80</v>
@@ -31380,13 +31383,13 @@
         <v>70</v>
       </c>
       <c r="AA3" s="22">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AB3" s="22">
         <v>70</v>
       </c>
       <c r="AC3" s="34">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AD3" s="34">
         <v>70</v>
@@ -31498,7 +31501,7 @@
       </c>
       <c r="AA4" s="22">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AB4" s="22">
         <f t="shared" si="0"/>
@@ -31506,7 +31509,7 @@
       </c>
       <c r="AC4" s="34">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AD4" s="34">
         <f t="shared" ref="AD4" si="5">(AD2+AD3)/2</f>
@@ -31593,13 +31596,13 @@
         <v>80</v>
       </c>
       <c r="AA5" s="22">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AB5" s="22">
         <v>80</v>
       </c>
       <c r="AC5" s="34">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AD5" s="34">
         <v>80</v>
@@ -31685,13 +31688,13 @@
         <v>70</v>
       </c>
       <c r="AA6" s="40">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AB6" s="40">
         <v>70</v>
       </c>
       <c r="AC6" s="40">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="AD6" s="40">
         <v>70</v>
@@ -31803,7 +31806,7 @@
       </c>
       <c r="AA7" s="32">
         <f t="shared" si="6"/>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AB7" s="32">
         <f t="shared" si="6"/>
@@ -31811,7 +31814,7 @@
       </c>
       <c r="AC7" s="32">
         <f t="shared" si="6"/>
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="AD7" s="32">
         <f t="shared" ref="AD7" si="11">(AD5+AD6)/2</f>
@@ -32209,7 +32212,7 @@
         <v>30</v>
       </c>
       <c r="AC11" s="32">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AD11" s="32">
         <v>30</v>
@@ -32301,7 +32304,7 @@
         <v>20</v>
       </c>
       <c r="AC12" s="32">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="AD12" s="32">
         <v>20</v>
@@ -32421,7 +32424,7 @@
       </c>
       <c r="AC13" s="32">
         <f t="shared" si="18"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AD13" s="32">
         <f t="shared" ref="AD13" si="23">(AD11+AD12)/2</f>

</xml_diff>

<commit_message>
add Necromance Bone Master and Skeleton Mage
</commit_message>
<xml_diff>
--- a/data/Hero_basic_property.xlsx
+++ b/data/Hero_basic_property.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Projects\Legends of Champions Tactics_Git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5347AA2E-D7C6-4CF6-8620-0A58389C45A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D5A8CF-D762-4007-BF6C-C3EE83DC7B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Warrior</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Mage_Skeleton</t>
+  </si>
+  <si>
+    <t>Necromancer_Bone_Master</t>
   </si>
 </sst>
 </file>
@@ -2407,27 +2410,27 @@
         <v>85</v>
       </c>
       <c r="H8" s="22">
-        <f>'Property List'!U4</f>
+        <f>'Property List'!V4</f>
         <v>95</v>
       </c>
       <c r="I8" s="22">
-        <f>'Property List'!X4</f>
+        <f>'Property List'!Y4</f>
         <v>105</v>
       </c>
       <c r="J8" s="22">
-        <f>'Property List'!AA4</f>
+        <f>'Property List'!AB4</f>
         <v>75</v>
       </c>
       <c r="K8" s="22">
-        <f>'Property List'!AB4</f>
+        <f>'Property List'!AC4</f>
         <v>70</v>
       </c>
       <c r="L8" s="22">
-        <f>'Property List'!AC4</f>
+        <f>'Property List'!AD4</f>
         <v>75</v>
       </c>
       <c r="M8" s="22">
-        <f>'Property List'!AD4</f>
+        <f>'Property List'!AE4</f>
         <v>80</v>
       </c>
       <c r="N8" s="13">
@@ -2475,27 +2478,27 @@
         <v>65</v>
       </c>
       <c r="H9" s="22">
-        <f>'Property List'!U7</f>
+        <f>'Property List'!V7</f>
         <v>70</v>
       </c>
       <c r="I9" s="22">
-        <f>'Property List'!X7</f>
+        <f>'Property List'!Y7</f>
         <v>65</v>
       </c>
       <c r="J9" s="22">
-        <f>'Property List'!AA7</f>
+        <f>'Property List'!AB7</f>
         <v>75</v>
       </c>
       <c r="K9" s="22">
-        <f>'Property List'!AB7</f>
+        <f>'Property List'!AC7</f>
         <v>80</v>
       </c>
       <c r="L9" s="22">
-        <f>'Property List'!AC7</f>
+        <f>'Property List'!AD7</f>
         <v>75</v>
       </c>
       <c r="M9" s="22">
-        <f>'Property List'!AD7</f>
+        <f>'Property List'!AE7</f>
         <v>65</v>
       </c>
       <c r="N9" s="13">
@@ -2543,27 +2546,27 @@
         <v>32</v>
       </c>
       <c r="H10" s="22">
-        <f>'Property List'!U10</f>
+        <f>'Property List'!V10</f>
         <v>27</v>
       </c>
       <c r="I10" s="22">
-        <f>'Property List'!X10</f>
+        <f>'Property List'!Y10</f>
         <v>50</v>
       </c>
       <c r="J10" s="22">
-        <f>'Property List'!AA10</f>
-        <v>27</v>
-      </c>
-      <c r="K10" s="22">
         <f>'Property List'!AB10</f>
         <v>27</v>
       </c>
-      <c r="L10" s="22">
+      <c r="K10" s="22">
         <f>'Property List'!AC10</f>
         <v>27</v>
       </c>
+      <c r="L10" s="22">
+        <f>'Property List'!AD10</f>
+        <v>27</v>
+      </c>
       <c r="M10" s="22">
-        <f>'Property List'!AD10</f>
+        <f>'Property List'!AE10</f>
         <v>27</v>
       </c>
       <c r="N10" s="13">
@@ -2611,27 +2614,27 @@
         <v>30</v>
       </c>
       <c r="H11" s="22">
-        <f>'Property List'!U13</f>
+        <f>'Property List'!V13</f>
         <v>25</v>
       </c>
       <c r="I11" s="22">
-        <f>'Property List'!X13</f>
+        <f>'Property List'!Y13</f>
         <v>15</v>
       </c>
       <c r="J11" s="22">
-        <f>'Property List'!AA13</f>
-        <v>25</v>
-      </c>
-      <c r="K11" s="22">
         <f>'Property List'!AB13</f>
         <v>25</v>
       </c>
-      <c r="L11" s="22">
+      <c r="K11" s="22">
         <f>'Property List'!AC13</f>
         <v>25</v>
       </c>
+      <c r="L11" s="22">
+        <f>'Property List'!AD13</f>
+        <v>25</v>
+      </c>
       <c r="M11" s="22">
-        <f>'Property List'!AD13</f>
+        <f>'Property List'!AE13</f>
         <v>30</v>
       </c>
       <c r="N11" s="13">
@@ -2679,27 +2682,27 @@
         <v>34</v>
       </c>
       <c r="H12" s="21">
-        <f>'Property List'!U17</f>
+        <f>'Property List'!V17</f>
         <v>34</v>
       </c>
       <c r="I12" s="21">
-        <f>'Property List'!X17</f>
+        <f>'Property List'!Y17</f>
         <v>31</v>
       </c>
       <c r="J12" s="21">
-        <f>'Property List'!AA17</f>
-        <v>34</v>
-      </c>
-      <c r="K12" s="21">
         <f>'Property List'!AB17</f>
         <v>34</v>
       </c>
-      <c r="L12" s="21">
+      <c r="K12" s="21">
         <f>'Property List'!AC17</f>
         <v>34</v>
       </c>
+      <c r="L12" s="21">
+        <f>'Property List'!AD17</f>
+        <v>34</v>
+      </c>
       <c r="M12" s="21">
-        <f>'Property List'!AD17</f>
+        <f>'Property List'!AE17</f>
         <v>34</v>
       </c>
       <c r="N12" s="13">
@@ -30394,13 +30397,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF1000"/>
+  <dimension ref="A1:AG1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30415,7 +30418,7 @@
     <col min="16" max="19" width="31" customWidth="1"/>
     <col min="20" max="20" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="26.21875" customWidth="1"/>
-    <col min="22" max="22" width="16.21875" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" customWidth="1"/>
     <col min="23" max="23" width="19.44140625" customWidth="1"/>
     <col min="24" max="24" width="18.21875" customWidth="1"/>
     <col min="25" max="26" width="19.6640625" customWidth="1"/>
@@ -30424,7 +30427,7 @@
     <col min="32" max="32" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>17</v>
@@ -30483,44 +30486,47 @@
       <c r="T1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" s="24" t="s">
+      <c r="AB1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AC1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="AC1" s="24" t="s">
+      <c r="AD1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="AD1" s="24" t="s">
+      <c r="AE1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AE1" s="24" t="s">
+      <c r="AF1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>42</v>
       </c>
@@ -30581,8 +30587,8 @@
       <c r="T2" s="26">
         <v>90</v>
       </c>
-      <c r="U2" s="27">
-        <v>100</v>
+      <c r="U2" s="26">
+        <v>90</v>
       </c>
       <c r="V2" s="27">
         <v>100</v>
@@ -30591,34 +30597,37 @@
         <v>100</v>
       </c>
       <c r="X2" s="27">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Y2" s="27">
         <v>110</v>
       </c>
-      <c r="Z2" s="28">
+      <c r="Z2" s="27">
         <v>110</v>
       </c>
-      <c r="AA2" s="21">
+      <c r="AA2" s="28">
+        <v>110</v>
+      </c>
+      <c r="AB2" s="21">
         <v>80</v>
       </c>
-      <c r="AB2" s="21">
+      <c r="AC2" s="21">
         <v>75</v>
       </c>
-      <c r="AC2" s="21">
+      <c r="AD2" s="21">
         <v>80</v>
       </c>
-      <c r="AD2" s="29">
+      <c r="AE2" s="29">
         <v>85</v>
       </c>
-      <c r="AE2" s="29">
+      <c r="AF2" s="29">
         <v>80</v>
       </c>
-      <c r="AF2" s="21">
+      <c r="AG2" s="21">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>43</v>
       </c>
@@ -30679,8 +30688,8 @@
       <c r="T3" s="31">
         <v>80</v>
       </c>
-      <c r="U3" s="32">
-        <v>90</v>
+      <c r="U3" s="31">
+        <v>80</v>
       </c>
       <c r="V3" s="32">
         <v>90</v>
@@ -30689,39 +30698,42 @@
         <v>90</v>
       </c>
       <c r="X3" s="32">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Y3" s="32">
         <v>100</v>
       </c>
-      <c r="Z3" s="33">
+      <c r="Z3" s="32">
         <v>100</v>
       </c>
-      <c r="AA3" s="21">
+      <c r="AA3" s="33">
+        <v>100</v>
+      </c>
+      <c r="AB3" s="21">
         <v>70</v>
       </c>
-      <c r="AB3" s="21">
+      <c r="AC3" s="21">
         <v>65</v>
       </c>
-      <c r="AC3" s="21">
+      <c r="AD3" s="21">
         <v>70</v>
       </c>
-      <c r="AD3" s="29">
+      <c r="AE3" s="29">
         <v>75</v>
       </c>
-      <c r="AE3" s="29">
+      <c r="AF3" s="29">
         <v>70</v>
       </c>
-      <c r="AF3" s="21">
+      <c r="AG3" s="21">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="21">
-        <f t="shared" ref="B4:AE4" si="0">(B2+B3)/2</f>
+        <f t="shared" ref="B4:AF4" si="0">(B2+B3)/2</f>
         <v>100</v>
       </c>
       <c r="C4" s="21">
@@ -30797,8 +30809,8 @@
         <v>85</v>
       </c>
       <c r="U4" s="21">
-        <f t="shared" si="0"/>
-        <v>95</v>
+        <f t="shared" ref="U4" si="1">(U2+U3)/2</f>
+        <v>85</v>
       </c>
       <c r="V4" s="21">
         <f t="shared" si="0"/>
@@ -30810,7 +30822,7 @@
       </c>
       <c r="X4" s="21">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="Y4" s="21">
         <f t="shared" si="0"/>
@@ -30822,30 +30834,34 @@
       </c>
       <c r="AA4" s="21">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="AB4" s="21">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AC4" s="21">
         <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="AD4" s="21">
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="AD4" s="29">
+      <c r="AE4" s="29">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="AE4" s="29">
+      <c r="AF4" s="29">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="AF4" s="21">
-        <f t="shared" ref="AF4" si="1">(AF2+AF3)/2</f>
+      <c r="AG4" s="21">
+        <f t="shared" ref="AG4" si="2">(AG2+AG3)/2</f>
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>44</v>
       </c>
@@ -30906,8 +30922,8 @@
       <c r="T5" s="34">
         <v>70</v>
       </c>
-      <c r="U5" s="35">
-        <v>75</v>
+      <c r="U5" s="34">
+        <v>70</v>
       </c>
       <c r="V5" s="35">
         <v>75</v>
@@ -30916,34 +30932,37 @@
         <v>75</v>
       </c>
       <c r="X5" s="35">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Y5" s="35">
         <v>70</v>
       </c>
-      <c r="Z5" s="36">
+      <c r="Z5" s="35">
         <v>70</v>
       </c>
-      <c r="AA5" s="21">
+      <c r="AA5" s="36">
+        <v>70</v>
+      </c>
+      <c r="AB5" s="21">
         <v>80</v>
       </c>
-      <c r="AB5" s="21">
+      <c r="AC5" s="21">
         <v>85</v>
       </c>
-      <c r="AC5" s="21">
+      <c r="AD5" s="21">
         <v>80</v>
       </c>
-      <c r="AD5" s="29">
+      <c r="AE5" s="29">
         <v>70</v>
       </c>
-      <c r="AE5" s="29">
+      <c r="AF5" s="29">
         <v>80</v>
       </c>
-      <c r="AF5" s="21">
+      <c r="AG5" s="21">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>45</v>
       </c>
@@ -31005,7 +31024,7 @@
         <v>60</v>
       </c>
       <c r="U6" s="27">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="V6" s="27">
         <v>65</v>
@@ -31014,7 +31033,7 @@
         <v>65</v>
       </c>
       <c r="X6" s="27">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="Y6" s="27">
         <v>60</v>
@@ -31022,155 +31041,162 @@
       <c r="Z6" s="27">
         <v>60</v>
       </c>
-      <c r="AA6" s="35">
+      <c r="AA6" s="27">
+        <v>60</v>
+      </c>
+      <c r="AB6" s="35">
         <v>70</v>
       </c>
-      <c r="AB6" s="35">
+      <c r="AC6" s="35">
         <v>75</v>
       </c>
-      <c r="AC6" s="35">
+      <c r="AD6" s="35">
         <v>70</v>
       </c>
-      <c r="AD6" s="35">
+      <c r="AE6" s="35">
         <v>60</v>
       </c>
-      <c r="AE6" s="35">
+      <c r="AF6" s="35">
         <v>70</v>
       </c>
-      <c r="AF6" s="34">
+      <c r="AG6" s="34">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="26">
-        <f t="shared" ref="B7:AE7" si="2">(B5+B6)/2</f>
+        <f t="shared" ref="B7:AF7" si="3">(B5+B6)/2</f>
         <v>70</v>
       </c>
       <c r="C7" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="D7" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="E7" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="F7" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="G7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="H7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="I7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="J7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="K7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="L7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="M7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="N7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="O7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="P7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="Q7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="R7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="S7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="T7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="U7" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="U7" si="4">(U5+U6)/2</f>
+        <v>65</v>
+      </c>
+      <c r="V7" s="27">
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="V7" s="27">
-        <f t="shared" si="2"/>
+      <c r="W7" s="27">
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="W7" s="27">
-        <f t="shared" si="2"/>
+      <c r="X7" s="27">
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="X7" s="27">
-        <f t="shared" si="2"/>
+      <c r="Y7" s="27">
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="Y7" s="27">
-        <f t="shared" si="2"/>
+      <c r="Z7" s="27">
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="Z7" s="27">
-        <f t="shared" si="2"/>
+      <c r="AA7" s="27">
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="AA7" s="27">
-        <f t="shared" si="2"/>
+      <c r="AB7" s="27">
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="AB7" s="27">
-        <f t="shared" si="2"/>
+      <c r="AC7" s="27">
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="AC7" s="27">
-        <f t="shared" si="2"/>
+      <c r="AD7" s="27">
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="AD7" s="27">
-        <f t="shared" si="2"/>
+      <c r="AE7" s="27">
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="AE7" s="27">
-        <f t="shared" si="2"/>
+      <c r="AF7" s="27">
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="AF7" s="26">
-        <f t="shared" ref="AF7" si="3">(AF5+AF6)/2</f>
+      <c r="AG7" s="26">
+        <f t="shared" ref="AG7" si="5">(AG5+AG6)/2</f>
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>46</v>
       </c>
@@ -31232,7 +31258,7 @@
         <v>35</v>
       </c>
       <c r="U8" s="27">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="V8" s="27">
         <v>30</v>
@@ -31241,7 +31267,7 @@
         <v>30</v>
       </c>
       <c r="X8" s="27">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="Y8" s="27">
         <v>55</v>
@@ -31250,7 +31276,7 @@
         <v>55</v>
       </c>
       <c r="AA8" s="27">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="AB8" s="27">
         <v>30</v>
@@ -31264,11 +31290,14 @@
       <c r="AE8" s="27">
         <v>30</v>
       </c>
-      <c r="AF8" s="26">
+      <c r="AF8" s="27">
+        <v>30</v>
+      </c>
+      <c r="AG8" s="26">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>47</v>
       </c>
@@ -31330,7 +31359,7 @@
         <v>29</v>
       </c>
       <c r="U9" s="27">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="V9" s="27">
         <v>24</v>
@@ -31339,7 +31368,7 @@
         <v>24</v>
       </c>
       <c r="X9" s="27">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="Y9" s="27">
         <v>45</v>
@@ -31348,7 +31377,7 @@
         <v>45</v>
       </c>
       <c r="AA9" s="27">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="AB9" s="27">
         <v>24</v>
@@ -31362,140 +31391,147 @@
       <c r="AE9" s="27">
         <v>24</v>
       </c>
-      <c r="AF9" s="26">
+      <c r="AF9" s="27">
+        <v>24</v>
+      </c>
+      <c r="AG9" s="26">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="26">
-        <f t="shared" ref="B10:AE10" si="4">(B8+B9)/2</f>
+        <f t="shared" ref="B10:AF10" si="6">(B8+B9)/2</f>
         <v>45</v>
       </c>
       <c r="C10" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="D10" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="E10" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="F10" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="G10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="H10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="I10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="J10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="K10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="L10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="M10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="N10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="O10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="P10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="Q10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="R10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="S10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="T10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="U10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="U10" si="7">(U8+U9)/2</f>
+        <v>32</v>
+      </c>
+      <c r="V10" s="27">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="V10" s="27">
-        <f t="shared" si="4"/>
+      <c r="W10" s="27">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="W10" s="27">
-        <f t="shared" si="4"/>
+      <c r="X10" s="27">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="X10" s="27">
-        <f t="shared" si="4"/>
+      <c r="Y10" s="27">
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="Y10" s="27">
-        <f t="shared" si="4"/>
+      <c r="Z10" s="27">
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="Z10" s="27">
-        <f t="shared" si="4"/>
+      <c r="AA10" s="27">
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="AA10" s="27">
-        <f t="shared" si="4"/>
+      <c r="AB10" s="27">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="AB10" s="27">
-        <f t="shared" si="4"/>
+      <c r="AC10" s="27">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="AC10" s="27">
-        <f t="shared" si="4"/>
+      <c r="AD10" s="27">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="AD10" s="27">
-        <f t="shared" si="4"/>
+      <c r="AE10" s="27">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="AE10" s="27">
-        <f t="shared" si="4"/>
+      <c r="AF10" s="27">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="AF10" s="26">
-        <f t="shared" ref="AF10" si="5">(AF8+AF9)/2</f>
+      <c r="AG10" s="26">
+        <f t="shared" ref="AG10" si="8">(AG8+AG9)/2</f>
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>48</v>
       </c>
@@ -31557,7 +31593,7 @@
         <v>35</v>
       </c>
       <c r="U11" s="27">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="V11" s="27">
         <v>30</v>
@@ -31566,7 +31602,7 @@
         <v>30</v>
       </c>
       <c r="X11" s="27">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="Y11" s="27">
         <v>20</v>
@@ -31575,7 +31611,7 @@
         <v>20</v>
       </c>
       <c r="AA11" s="27">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="AB11" s="27">
         <v>30</v>
@@ -31584,16 +31620,19 @@
         <v>30</v>
       </c>
       <c r="AD11" s="27">
+        <v>30</v>
+      </c>
+      <c r="AE11" s="27">
         <v>35</v>
       </c>
-      <c r="AE11" s="27">
+      <c r="AF11" s="27">
         <v>30</v>
       </c>
-      <c r="AF11" s="26">
+      <c r="AG11" s="26">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>49</v>
       </c>
@@ -31655,7 +31694,7 @@
         <v>25</v>
       </c>
       <c r="U12" s="27">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="V12" s="27">
         <v>20</v>
@@ -31664,7 +31703,7 @@
         <v>20</v>
       </c>
       <c r="X12" s="27">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Y12" s="27">
         <v>10</v>
@@ -31673,7 +31712,7 @@
         <v>10</v>
       </c>
       <c r="AA12" s="27">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AB12" s="27">
         <v>20</v>
@@ -31682,145 +31721,152 @@
         <v>20</v>
       </c>
       <c r="AD12" s="27">
+        <v>20</v>
+      </c>
+      <c r="AE12" s="27">
         <v>25</v>
       </c>
-      <c r="AE12" s="27">
+      <c r="AF12" s="27">
         <v>20</v>
       </c>
-      <c r="AF12" s="26">
+      <c r="AG12" s="26">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="26">
-        <f t="shared" ref="B13:AE13" si="6">(B11+B12)/2</f>
+        <f t="shared" ref="B13:AF13" si="9">(B11+B12)/2</f>
         <v>25</v>
       </c>
       <c r="C13" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="D13" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="E13" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="F13" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="G13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="H13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="I13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="K13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="L13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="M13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="N13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="O13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="P13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="Q13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="R13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="S13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="T13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="U13" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="U13" si="10">(U11+U12)/2</f>
+        <v>30</v>
+      </c>
+      <c r="V13" s="27">
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="V13" s="27">
-        <f t="shared" si="6"/>
+      <c r="W13" s="27">
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="W13" s="27">
-        <f t="shared" si="6"/>
+      <c r="X13" s="27">
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="X13" s="27">
-        <f t="shared" si="6"/>
+      <c r="Y13" s="27">
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
-      <c r="Y13" s="27">
-        <f t="shared" si="6"/>
+      <c r="Z13" s="27">
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
-      <c r="Z13" s="27">
-        <f t="shared" si="6"/>
+      <c r="AA13" s="27">
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
-      <c r="AA13" s="27">
-        <f t="shared" si="6"/>
+      <c r="AB13" s="27">
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="AB13" s="27">
-        <f t="shared" si="6"/>
+      <c r="AC13" s="27">
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="AC13" s="27">
-        <f t="shared" si="6"/>
+      <c r="AD13" s="27">
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="AD13" s="27">
-        <f t="shared" si="6"/>
+      <c r="AE13" s="27">
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
-      <c r="AE13" s="27">
-        <f t="shared" si="6"/>
+      <c r="AF13" s="27">
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="AF13" s="26">
-        <f t="shared" ref="AF13" si="7">(AF11+AF12)/2</f>
+      <c r="AG13" s="26">
+        <f t="shared" ref="AG13" si="11">(AG11+AG12)/2</f>
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>50</v>
       </c>
@@ -31914,11 +31960,14 @@
       <c r="AE14" s="27">
         <v>5</v>
       </c>
-      <c r="AF14" s="26">
+      <c r="AF14" s="27">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG14" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>51</v>
       </c>
@@ -32012,140 +32061,147 @@
       <c r="AE15" s="27">
         <v>-5</v>
       </c>
-      <c r="AF15" s="26">
+      <c r="AF15" s="27">
         <v>-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG15" s="26">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="26">
-        <f t="shared" ref="B16:AE16" si="8">(B14+B15)/2</f>
+        <f t="shared" ref="B16:AF16" si="12">(B14+B15)/2</f>
         <v>0</v>
       </c>
       <c r="C16" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="D16" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E16" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F16" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="R16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="U16" si="13">(U14+U15)/2</f>
         <v>0</v>
       </c>
       <c r="V16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Y16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Z16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AA16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AB16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AC16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE16" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF16" s="26">
-        <f t="shared" ref="AF16" si="9">(AF14+AF15)/2</f>
+      <c r="AF16" s="27">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG16" s="26">
+        <f t="shared" ref="AG16" si="14">(AG14+AG15)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>16</v>
       </c>
@@ -32216,7 +32272,7 @@
         <v>34</v>
       </c>
       <c r="X17" s="27">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Y17" s="27">
         <v>31</v>
@@ -32225,7 +32281,7 @@
         <v>31</v>
       </c>
       <c r="AA17" s="27">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AB17" s="27">
         <v>34</v>
@@ -32239,11 +32295,14 @@
       <c r="AE17" s="27">
         <v>34</v>
       </c>
-      <c r="AF17" s="26">
+      <c r="AF17" s="27">
+        <v>34</v>
+      </c>
+      <c r="AG17" s="26">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="37"/>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
@@ -32276,137 +32335,142 @@
       <c r="AD18" s="27"/>
       <c r="AE18" s="27"/>
       <c r="AF18" s="27"/>
-    </row>
-    <row r="19" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG18" s="27"/>
+    </row>
+    <row r="19" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="27">
-        <f t="shared" ref="B19:AE19" si="10">B4+B7+B10+B13+B16+B17</f>
+        <f t="shared" ref="B19:AF19" si="15">B4+B7+B10+B13+B16+B17</f>
         <v>265</v>
       </c>
       <c r="C19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>265</v>
       </c>
       <c r="D19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>265</v>
       </c>
       <c r="E19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>265</v>
       </c>
       <c r="F19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>204</v>
       </c>
       <c r="G19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>199</v>
       </c>
       <c r="H19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>204</v>
       </c>
       <c r="I19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>266</v>
       </c>
       <c r="J19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>266</v>
       </c>
       <c r="K19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>266</v>
       </c>
       <c r="L19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>261</v>
       </c>
       <c r="M19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>261</v>
       </c>
       <c r="N19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>261</v>
       </c>
       <c r="O19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>244</v>
       </c>
       <c r="P19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>244</v>
       </c>
       <c r="Q19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>244</v>
       </c>
       <c r="R19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>244</v>
       </c>
       <c r="S19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>244</v>
       </c>
       <c r="T19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>246</v>
       </c>
       <c r="U19" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="U19" si="16">U4+U7+U10+U13+U16+U17</f>
+        <v>246</v>
+      </c>
+      <c r="V19" s="27">
+        <f t="shared" si="15"/>
         <v>251</v>
       </c>
-      <c r="V19" s="27">
-        <f t="shared" si="10"/>
+      <c r="W19" s="27">
+        <f t="shared" si="15"/>
         <v>251</v>
       </c>
-      <c r="W19" s="27">
-        <f t="shared" si="10"/>
+      <c r="X19" s="27">
+        <f t="shared" si="15"/>
         <v>251</v>
       </c>
-      <c r="X19" s="27">
-        <f t="shared" si="10"/>
+      <c r="Y19" s="27">
+        <f t="shared" si="15"/>
         <v>266</v>
       </c>
-      <c r="Y19" s="27">
-        <f t="shared" si="10"/>
+      <c r="Z19" s="27">
+        <f t="shared" si="15"/>
         <v>266</v>
       </c>
-      <c r="Z19" s="27">
-        <f t="shared" si="10"/>
+      <c r="AA19" s="27">
+        <f t="shared" si="15"/>
         <v>266</v>
       </c>
-      <c r="AA19" s="27">
-        <f t="shared" si="10"/>
+      <c r="AB19" s="27">
+        <f t="shared" si="15"/>
         <v>236</v>
       </c>
-      <c r="AB19" s="27">
-        <f t="shared" si="10"/>
+      <c r="AC19" s="27">
+        <f t="shared" si="15"/>
         <v>236</v>
       </c>
-      <c r="AC19" s="27">
-        <f t="shared" si="10"/>
+      <c r="AD19" s="27">
+        <f t="shared" si="15"/>
         <v>236</v>
       </c>
-      <c r="AD19" s="27">
-        <f t="shared" si="10"/>
+      <c r="AE19" s="27">
+        <f t="shared" si="15"/>
         <v>236</v>
       </c>
-      <c r="AE19" s="27">
-        <f t="shared" si="10"/>
+      <c r="AF19" s="27">
+        <f t="shared" si="15"/>
         <v>236</v>
       </c>
-      <c r="AF19" s="27">
-        <f t="shared" ref="AF19" si="11">AF4+AF7+AF10+AF13+AF16+AF17</f>
+      <c r="AG19" s="27">
+        <f t="shared" ref="AG19" si="17">AG4+AG7+AG10+AG13+AG16+AG17</f>
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -32440,7 +32504,7 @@
       <c r="AE20" s="23"/>
       <c r="AF20" s="23"/>
     </row>
-    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
@@ -32474,7 +32538,7 @@
       <c r="AE21" s="23"/>
       <c r="AF21" s="23"/>
     </row>
-    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -32508,7 +32572,7 @@
       <c r="AE22" s="23"/>
       <c r="AF22" s="23"/>
     </row>
-    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -32542,7 +32606,7 @@
       <c r="AE23" s="23"/>
       <c r="AF23" s="23"/>
     </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -32576,7 +32640,7 @@
       <c r="AE24" s="23"/>
       <c r="AF24" s="23"/>
     </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -32610,7 +32674,7 @@
       <c r="AE25" s="23"/>
       <c r="AF25" s="23"/>
     </row>
-    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
@@ -32644,7 +32708,7 @@
       <c r="AE26" s="23"/>
       <c r="AF26" s="23"/>
     </row>
-    <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -32678,7 +32742,7 @@
       <c r="AE27" s="23"/>
       <c r="AF27" s="23"/>
     </row>
-    <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -32712,7 +32776,7 @@
       <c r="AE28" s="23"/>
       <c r="AF28" s="23"/>
     </row>
-    <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="23"/>
       <c r="C29" s="23"/>
@@ -32746,7 +32810,7 @@
       <c r="AE29" s="23"/>
       <c r="AF29" s="23"/>
     </row>
-    <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
@@ -32780,7 +32844,7 @@
       <c r="AE30" s="23"/>
       <c r="AF30" s="23"/>
     </row>
-    <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -32814,7 +32878,7 @@
       <c r="AE31" s="23"/>
       <c r="AF31" s="23"/>
     </row>
-    <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="23"/>
       <c r="C32" s="23"/>

</xml_diff>